<commit_message>
updated book list and blueprint topics
</commit_message>
<xml_diff>
--- a/blueprints-combined.xlsx
+++ b/blueprints-combined.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qdd/Google Drive/git/notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C34227-97D4-EA4D-AA5E-A158EFCDA3FC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C63146-553F-1842-9526-B6EE6327AA87}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11700" yWindow="1580" windowWidth="26140" windowHeight="19420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11580" yWindow="1500" windowWidth="26140" windowHeight="19420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lab-topics" sheetId="6" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1744" uniqueCount="952">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1760" uniqueCount="952">
   <si>
     <t>date</t>
   </si>
@@ -3577,7 +3578,14 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3587,6 +3595,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3607,32 +3639,17 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3643,31 +3660,15 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -4150,10 +4151,10 @@
   <dimension ref="A1:P349"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C287" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B65" sqref="B65"/>
+      <selection pane="bottomRight" activeCell="B305" sqref="B305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4176,7 +4177,7 @@
       </c>
       <c r="F1" s="90">
         <f ca="1">(TODAY()-H1)*-1</f>
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="G1" s="91" t="s">
         <v>10</v>
@@ -4501,7 +4502,7 @@
       <c r="B37" s="7" t="s">
         <v>626</v>
       </c>
-      <c r="C37" s="128"/>
+      <c r="C37" s="98"/>
     </row>
     <row r="38" spans="1:3" ht="16">
       <c r="A38" s="83" t="s">
@@ -4510,7 +4511,7 @@
       <c r="B38" s="7" t="s">
         <v>627</v>
       </c>
-      <c r="C38" s="128"/>
+      <c r="C38" s="98"/>
     </row>
     <row r="39" spans="1:3" ht="16">
       <c r="A39" s="83" t="s">
@@ -4519,7 +4520,7 @@
       <c r="B39" s="7" t="s">
         <v>628</v>
       </c>
-      <c r="C39" s="128"/>
+      <c r="C39" s="98"/>
     </row>
     <row r="40" spans="1:3" ht="19">
       <c r="A40" s="83" t="s">
@@ -4690,6 +4691,9 @@
       <c r="B60" s="7" t="s">
         <v>650</v>
       </c>
+      <c r="C60" t="s">
+        <v>951</v>
+      </c>
     </row>
     <row r="61" spans="1:4" ht="16">
       <c r="A61" s="83" t="s">
@@ -4698,6 +4702,9 @@
       <c r="B61" s="7" t="s">
         <v>651</v>
       </c>
+      <c r="C61" t="s">
+        <v>951</v>
+      </c>
     </row>
     <row r="62" spans="1:4" ht="16">
       <c r="A62" s="83" t="s">
@@ -4706,6 +4713,9 @@
       <c r="B62" s="7" t="s">
         <v>652</v>
       </c>
+      <c r="C62" t="s">
+        <v>951</v>
+      </c>
     </row>
     <row r="63" spans="1:4" ht="16">
       <c r="A63" s="83" t="s">
@@ -4714,6 +4724,9 @@
       <c r="B63" s="7" t="s">
         <v>653</v>
       </c>
+      <c r="C63" t="s">
+        <v>951</v>
+      </c>
     </row>
     <row r="64" spans="1:4" ht="16">
       <c r="A64" s="83" t="s">
@@ -4722,6 +4735,9 @@
       <c r="B64" s="7" t="s">
         <v>654</v>
       </c>
+      <c r="C64" t="s">
+        <v>951</v>
+      </c>
     </row>
     <row r="65" spans="1:4" ht="16">
       <c r="A65" s="83" t="s">
@@ -4730,6 +4746,9 @@
       <c r="B65" s="7" t="s">
         <v>655</v>
       </c>
+      <c r="C65" t="s">
+        <v>951</v>
+      </c>
     </row>
     <row r="66" spans="1:4" ht="16">
       <c r="A66" s="83" t="s">
@@ -4738,6 +4757,9 @@
       <c r="B66" s="7" t="s">
         <v>656</v>
       </c>
+      <c r="C66" t="s">
+        <v>951</v>
+      </c>
     </row>
     <row r="67" spans="1:4" ht="16">
       <c r="A67" s="83" t="s">
@@ -4746,6 +4768,9 @@
       <c r="B67" s="7" t="s">
         <v>657</v>
       </c>
+      <c r="C67" t="s">
+        <v>951</v>
+      </c>
     </row>
     <row r="68" spans="1:4" ht="16">
       <c r="A68" s="83" t="s">
@@ -4754,6 +4779,9 @@
       <c r="B68" s="7" t="s">
         <v>658</v>
       </c>
+      <c r="C68" t="s">
+        <v>951</v>
+      </c>
     </row>
     <row r="69" spans="1:4" ht="19">
       <c r="A69" s="83" t="s">
@@ -4905,7 +4933,7 @@
       <c r="B82" s="7" t="s">
         <v>671</v>
       </c>
-      <c r="C82" s="128"/>
+      <c r="C82" s="98"/>
     </row>
     <row r="83" spans="1:3" ht="19">
       <c r="A83" s="83" t="s">
@@ -5275,7 +5303,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="16">
+    <row r="129" spans="1:3" ht="16">
       <c r="A129" s="83" t="s">
         <v>929</v>
       </c>
@@ -5283,7 +5311,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="16">
+    <row r="130" spans="1:3" ht="16">
       <c r="A130" s="83" t="s">
         <v>929</v>
       </c>
@@ -5291,7 +5319,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="16">
+    <row r="131" spans="1:3" ht="16">
       <c r="A131" s="83" t="s">
         <v>929</v>
       </c>
@@ -5299,7 +5327,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="16">
+    <row r="132" spans="1:3" ht="16">
       <c r="A132" s="83" t="s">
         <v>929</v>
       </c>
@@ -5307,7 +5335,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="16">
+    <row r="133" spans="1:3" ht="16">
       <c r="A133" s="83" t="s">
         <v>929</v>
       </c>
@@ -5315,7 +5343,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="16">
+    <row r="134" spans="1:3" ht="16">
       <c r="A134" s="83" t="s">
         <v>929</v>
       </c>
@@ -5323,7 +5351,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="16">
+    <row r="135" spans="1:3" ht="16">
       <c r="A135" s="83" t="s">
         <v>929</v>
       </c>
@@ -5331,15 +5359,18 @@
         <v>720</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="16">
+    <row r="136" spans="1:3" ht="16">
       <c r="A136" s="83" t="s">
         <v>929</v>
       </c>
       <c r="B136" s="7" t="s">
         <v>721</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" ht="16">
+      <c r="C136" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="16">
       <c r="A137" s="83" t="s">
         <v>929</v>
       </c>
@@ -5347,7 +5378,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="16">
+    <row r="138" spans="1:3" ht="16">
       <c r="A138" s="83" t="s">
         <v>929</v>
       </c>
@@ -5355,7 +5386,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="16">
+    <row r="139" spans="1:3" ht="16">
       <c r="A139" s="83" t="s">
         <v>929</v>
       </c>
@@ -5363,7 +5394,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="16">
+    <row r="140" spans="1:3" ht="16">
       <c r="A140" s="83" t="s">
         <v>929</v>
       </c>
@@ -5371,7 +5402,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="16">
+    <row r="141" spans="1:3" ht="16">
       <c r="A141" s="83" t="s">
         <v>929</v>
       </c>
@@ -5379,7 +5410,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="16">
+    <row r="142" spans="1:3" ht="16">
       <c r="A142" s="83" t="s">
         <v>929</v>
       </c>
@@ -5387,7 +5418,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="19">
+    <row r="143" spans="1:3" ht="19">
       <c r="A143" s="83" t="s">
         <v>929</v>
       </c>
@@ -5395,7 +5426,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="16">
+    <row r="144" spans="1:3" ht="16">
       <c r="A144" s="83" t="s">
         <v>929</v>
       </c>
@@ -5403,15 +5434,18 @@
         <v>729</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="16">
+    <row r="145" spans="1:3" ht="16">
       <c r="A145" s="83" t="s">
         <v>929</v>
       </c>
       <c r="B145" s="7" t="s">
         <v>730</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" ht="16">
+      <c r="C145" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="16">
       <c r="A146" s="83" t="s">
         <v>929</v>
       </c>
@@ -5419,7 +5453,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="16">
+    <row r="147" spans="1:3" ht="16">
       <c r="A147" s="83" t="s">
         <v>929</v>
       </c>
@@ -5427,15 +5461,18 @@
         <v>732</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="16">
+    <row r="148" spans="1:3" ht="16">
       <c r="A148" s="83" t="s">
         <v>929</v>
       </c>
       <c r="B148" s="7" t="s">
         <v>733</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" ht="16">
+      <c r="C148" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="16">
       <c r="A149" s="83" t="s">
         <v>929</v>
       </c>
@@ -5443,7 +5480,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="16">
+    <row r="150" spans="1:3" ht="16">
       <c r="A150" s="83" t="s">
         <v>929</v>
       </c>
@@ -5451,7 +5488,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="16">
+    <row r="151" spans="1:3" ht="16">
       <c r="A151" s="83" t="s">
         <v>929</v>
       </c>
@@ -5459,7 +5496,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="16">
+    <row r="152" spans="1:3" ht="16">
       <c r="A152" s="83" t="s">
         <v>929</v>
       </c>
@@ -5467,7 +5504,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="16">
+    <row r="153" spans="1:3" ht="16">
       <c r="A153" s="83" t="s">
         <v>929</v>
       </c>
@@ -5475,7 +5512,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="16">
+    <row r="154" spans="1:3" ht="16">
       <c r="A154" s="83" t="s">
         <v>929</v>
       </c>
@@ -5483,7 +5520,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="16">
+    <row r="155" spans="1:3" ht="16">
       <c r="A155" s="83" t="s">
         <v>929</v>
       </c>
@@ -5491,7 +5528,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="16">
+    <row r="156" spans="1:3" ht="16">
       <c r="A156" s="83" t="s">
         <v>929</v>
       </c>
@@ -5499,7 +5536,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="16">
+    <row r="157" spans="1:3" ht="16">
       <c r="A157" s="83" t="s">
         <v>929</v>
       </c>
@@ -5507,7 +5544,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="16">
+    <row r="158" spans="1:3" ht="16">
       <c r="A158" s="83" t="s">
         <v>929</v>
       </c>
@@ -5515,7 +5552,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="16">
+    <row r="159" spans="1:3" ht="16">
       <c r="A159" s="83" t="s">
         <v>929</v>
       </c>
@@ -5523,7 +5560,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="16">
+    <row r="160" spans="1:3" ht="16">
       <c r="A160" s="83" t="s">
         <v>929</v>
       </c>
@@ -6561,7 +6598,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="289" spans="1:2" ht="16">
+    <row r="289" spans="1:3" ht="16">
       <c r="A289" s="83" t="s">
         <v>930</v>
       </c>
@@ -6569,7 +6606,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="290" spans="1:2" ht="16">
+    <row r="290" spans="1:3" ht="16">
       <c r="A290" s="83" t="s">
         <v>930</v>
       </c>
@@ -6577,7 +6614,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="291" spans="1:2" ht="16">
+    <row r="291" spans="1:3" ht="16">
       <c r="A291" s="83" t="s">
         <v>930</v>
       </c>
@@ -6585,7 +6622,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="292" spans="1:2" ht="16">
+    <row r="292" spans="1:3" ht="16">
       <c r="A292" s="83" t="s">
         <v>930</v>
       </c>
@@ -6593,7 +6630,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="293" spans="1:2" ht="16">
+    <row r="293" spans="1:3" ht="16">
       <c r="A293" s="83" t="s">
         <v>930</v>
       </c>
@@ -6601,7 +6638,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="294" spans="1:2" ht="16">
+    <row r="294" spans="1:3" ht="16">
       <c r="A294" s="83" t="s">
         <v>930</v>
       </c>
@@ -6609,7 +6646,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="295" spans="1:2" ht="16">
+    <row r="295" spans="1:3" ht="16">
       <c r="A295" s="83" t="s">
         <v>930</v>
       </c>
@@ -6617,7 +6654,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="296" spans="1:2" ht="16">
+    <row r="296" spans="1:3" ht="16">
       <c r="A296" s="83" t="s">
         <v>930</v>
       </c>
@@ -6625,7 +6662,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="297" spans="1:2" ht="16">
+    <row r="297" spans="1:3" ht="16">
       <c r="A297" s="83" t="s">
         <v>930</v>
       </c>
@@ -6633,7 +6670,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="298" spans="1:2" ht="19">
+    <row r="298" spans="1:3" ht="19">
       <c r="A298" s="83" t="s">
         <v>930</v>
       </c>
@@ -6641,7 +6678,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="299" spans="1:2" ht="16">
+    <row r="299" spans="1:3" ht="16">
       <c r="A299" s="83" t="s">
         <v>930</v>
       </c>
@@ -6649,39 +6686,51 @@
         <v>935</v>
       </c>
     </row>
-    <row r="300" spans="1:2" ht="16">
+    <row r="300" spans="1:3" ht="16">
       <c r="A300" s="83" t="s">
         <v>930</v>
       </c>
       <c r="B300" s="7" t="s">
         <v>878</v>
       </c>
-    </row>
-    <row r="301" spans="1:2" ht="16">
+      <c r="C300" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" ht="16">
       <c r="A301" s="83" t="s">
         <v>930</v>
       </c>
       <c r="B301" s="7" t="s">
         <v>879</v>
       </c>
-    </row>
-    <row r="302" spans="1:2" ht="16">
+      <c r="C301" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" ht="16">
       <c r="A302" s="83" t="s">
         <v>930</v>
       </c>
       <c r="B302" s="7" t="s">
         <v>880</v>
       </c>
-    </row>
-    <row r="303" spans="1:2" ht="16">
+      <c r="C302" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" ht="16">
       <c r="A303" s="83" t="s">
         <v>930</v>
       </c>
       <c r="B303" s="7" t="s">
         <v>881</v>
       </c>
-    </row>
-    <row r="304" spans="1:2" ht="16">
+      <c r="C303" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" ht="16">
       <c r="A304" s="83" t="s">
         <v>930</v>
       </c>
@@ -7115,10 +7164,10 @@
   <dimension ref="A1:P893"/>
   <sheetViews>
     <sheetView zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C287" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B298" sqref="B298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -7143,7 +7192,7 @@
       </c>
       <c r="F1" s="90">
         <f ca="1">(TODAY()-H1)*-1</f>
-        <v>-35</v>
+        <v>-49</v>
       </c>
       <c r="G1" s="91" t="s">
         <v>10</v>
@@ -14863,12 +14912,12 @@
       <c r="M1" s="16"/>
     </row>
     <row r="2" spans="1:13" s="18" customFormat="1" ht="26" customHeight="1">
-      <c r="A2" s="124"/>
-      <c r="B2" s="124"/>
-      <c r="C2" s="124"/>
-      <c r="D2" s="124"/>
-      <c r="E2" s="124"/>
-      <c r="F2" s="124"/>
+      <c r="A2" s="99"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
       <c r="G2" s="49" t="s">
         <v>501</v>
       </c>
@@ -14892,14 +14941,14 @@
       </c>
     </row>
     <row r="3" spans="1:13" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A3" s="125" t="s">
+      <c r="A3" s="100" t="s">
         <v>446</v>
       </c>
-      <c r="B3" s="126"/>
-      <c r="C3" s="126"/>
-      <c r="D3" s="126"/>
-      <c r="E3" s="126"/>
-      <c r="F3" s="126"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
       <c r="G3" s="27"/>
       <c r="H3" s="23"/>
       <c r="I3" s="24" t="s">
@@ -14910,12 +14959,12 @@
       <c r="M3" s="26"/>
     </row>
     <row r="4" spans="1:13" s="32" customFormat="1" ht="14" customHeight="1">
-      <c r="A4" s="126"/>
-      <c r="B4" s="126"/>
-      <c r="C4" s="126"/>
-      <c r="D4" s="126"/>
-      <c r="E4" s="126"/>
-      <c r="F4" s="126"/>
+      <c r="A4" s="101"/>
+      <c r="B4" s="101"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="101"/>
       <c r="G4" s="27"/>
       <c r="H4" s="27"/>
       <c r="I4" s="27"/>
@@ -14942,16 +14991,16 @@
       <c r="M5" s="40"/>
     </row>
     <row r="6" spans="1:13" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A6" s="99" t="s">
+      <c r="A6" s="102" t="s">
         <v>448</v>
       </c>
-      <c r="B6" s="99" t="s">
+      <c r="B6" s="102" t="s">
         <v>449</v>
       </c>
-      <c r="C6" s="99" t="s">
+      <c r="C6" s="102" t="s">
         <v>450</v>
       </c>
-      <c r="D6" s="114" t="s">
+      <c r="D6" s="106" t="s">
         <v>505</v>
       </c>
       <c r="E6" s="41" t="s">
@@ -14973,18 +15022,18 @@
       <c r="K6" s="43" t="s">
         <v>454</v>
       </c>
-      <c r="L6" s="111" t="s">
+      <c r="L6" s="110" t="s">
         <v>507</v>
       </c>
-      <c r="M6" s="111" t="s">
+      <c r="M6" s="110" t="s">
         <v>455</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A7" s="100"/>
-      <c r="B7" s="100"/>
-      <c r="C7" s="100"/>
-      <c r="D7" s="115"/>
+      <c r="A7" s="103"/>
+      <c r="B7" s="103"/>
+      <c r="C7" s="103"/>
+      <c r="D7" s="107"/>
       <c r="E7" s="41" t="s">
         <v>456</v>
       </c>
@@ -15006,22 +15055,22 @@
       <c r="K7" s="43" t="s">
         <v>458</v>
       </c>
-      <c r="L7" s="112"/>
-      <c r="M7" s="112"/>
+      <c r="L7" s="111"/>
+      <c r="M7" s="111"/>
     </row>
     <row r="8" spans="1:13" s="18" customFormat="1" ht="18" customHeight="1" outlineLevel="1">
-      <c r="A8" s="100"/>
-      <c r="B8" s="100"/>
-      <c r="C8" s="100"/>
-      <c r="D8" s="115"/>
-      <c r="E8" s="99" t="s">
+      <c r="A8" s="103"/>
+      <c r="B8" s="103"/>
+      <c r="C8" s="103"/>
+      <c r="D8" s="107"/>
+      <c r="E8" s="102" t="s">
         <v>459</v>
       </c>
-      <c r="F8" s="102" t="s">
+      <c r="F8" s="113" t="s">
         <v>511</v>
       </c>
       <c r="G8" s="78"/>
-      <c r="H8" s="105" t="s">
+      <c r="H8" s="116" t="s">
         <v>512</v>
       </c>
       <c r="I8" s="50" t="s">
@@ -15033,18 +15082,18 @@
       <c r="K8" s="43" t="s">
         <v>466</v>
       </c>
-      <c r="L8" s="112"/>
-      <c r="M8" s="112"/>
+      <c r="L8" s="111"/>
+      <c r="M8" s="111"/>
     </row>
     <row r="9" spans="1:13" s="18" customFormat="1" ht="16" customHeight="1" outlineLevel="1">
-      <c r="A9" s="100"/>
-      <c r="B9" s="100"/>
-      <c r="C9" s="100"/>
-      <c r="D9" s="115"/>
-      <c r="E9" s="100"/>
-      <c r="F9" s="103"/>
+      <c r="A9" s="103"/>
+      <c r="B9" s="103"/>
+      <c r="C9" s="103"/>
+      <c r="D9" s="107"/>
+      <c r="E9" s="103"/>
+      <c r="F9" s="114"/>
       <c r="G9" s="79"/>
-      <c r="H9" s="106"/>
+      <c r="H9" s="117"/>
       <c r="I9" s="50" t="s">
         <v>514</v>
       </c>
@@ -15052,41 +15101,41 @@
       <c r="K9" s="51" t="s">
         <v>515</v>
       </c>
-      <c r="L9" s="112"/>
-      <c r="M9" s="112"/>
+      <c r="L9" s="111"/>
+      <c r="M9" s="111"/>
     </row>
     <row r="10" spans="1:13" s="18" customFormat="1" ht="19" customHeight="1" outlineLevel="1">
-      <c r="A10" s="100"/>
-      <c r="B10" s="100"/>
-      <c r="C10" s="100"/>
-      <c r="D10" s="115"/>
-      <c r="E10" s="101"/>
-      <c r="F10" s="104"/>
+      <c r="A10" s="103"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="103"/>
+      <c r="D10" s="107"/>
+      <c r="E10" s="104"/>
+      <c r="F10" s="115"/>
       <c r="G10" s="58" t="s">
         <v>582</v>
       </c>
-      <c r="H10" s="107"/>
+      <c r="H10" s="118"/>
       <c r="I10" s="50" t="s">
         <v>516</v>
       </c>
       <c r="J10" s="44"/>
       <c r="K10" s="52"/>
-      <c r="L10" s="112"/>
-      <c r="M10" s="112"/>
+      <c r="L10" s="111"/>
+      <c r="M10" s="111"/>
     </row>
     <row r="11" spans="1:13" s="18" customFormat="1" ht="13" customHeight="1" outlineLevel="1">
-      <c r="A11" s="100"/>
-      <c r="B11" s="100"/>
-      <c r="C11" s="100"/>
-      <c r="D11" s="115"/>
-      <c r="E11" s="99" t="s">
+      <c r="A11" s="103"/>
+      <c r="B11" s="103"/>
+      <c r="C11" s="103"/>
+      <c r="D11" s="107"/>
+      <c r="E11" s="102" t="s">
         <v>461</v>
       </c>
-      <c r="F11" s="102" t="s">
+      <c r="F11" s="113" t="s">
         <v>517</v>
       </c>
       <c r="G11" s="78"/>
-      <c r="H11" s="98"/>
+      <c r="H11" s="120"/>
       <c r="I11" s="53" t="s">
         <v>518</v>
       </c>
@@ -15094,20 +15143,20 @@
       <c r="K11" s="43" t="s">
         <v>519</v>
       </c>
-      <c r="L11" s="112"/>
-      <c r="M11" s="112"/>
+      <c r="L11" s="111"/>
+      <c r="M11" s="111"/>
     </row>
     <row r="12" spans="1:13" s="18" customFormat="1" ht="18" customHeight="1" thickBot="1">
-      <c r="A12" s="100"/>
-      <c r="B12" s="100"/>
-      <c r="C12" s="120"/>
-      <c r="D12" s="127"/>
-      <c r="E12" s="120"/>
-      <c r="F12" s="121"/>
+      <c r="A12" s="103"/>
+      <c r="B12" s="103"/>
+      <c r="C12" s="105"/>
+      <c r="D12" s="108"/>
+      <c r="E12" s="105"/>
+      <c r="F12" s="119"/>
       <c r="G12" s="80" t="s">
         <v>582</v>
       </c>
-      <c r="H12" s="122"/>
+      <c r="H12" s="121"/>
       <c r="I12" s="54" t="s">
         <v>520</v>
       </c>
@@ -15115,16 +15164,16 @@
       <c r="K12" s="56" t="s">
         <v>521</v>
       </c>
-      <c r="L12" s="112"/>
-      <c r="M12" s="112"/>
+      <c r="L12" s="111"/>
+      <c r="M12" s="111"/>
     </row>
     <row r="13" spans="1:13" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A13" s="100"/>
-      <c r="B13" s="100"/>
-      <c r="C13" s="100" t="s">
+      <c r="A13" s="103"/>
+      <c r="B13" s="103"/>
+      <c r="C13" s="103" t="s">
         <v>462</v>
       </c>
-      <c r="D13" s="115" t="s">
+      <c r="D13" s="107" t="s">
         <v>522</v>
       </c>
       <c r="E13" s="57" t="s">
@@ -15146,14 +15195,14 @@
       <c r="K13" s="51" t="s">
         <v>526</v>
       </c>
-      <c r="L13" s="112"/>
-      <c r="M13" s="112"/>
+      <c r="L13" s="111"/>
+      <c r="M13" s="111"/>
     </row>
     <row r="14" spans="1:13" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A14" s="100"/>
-      <c r="B14" s="100"/>
-      <c r="C14" s="100"/>
-      <c r="D14" s="115"/>
+      <c r="A14" s="103"/>
+      <c r="B14" s="103"/>
+      <c r="C14" s="103"/>
+      <c r="D14" s="107"/>
       <c r="E14" s="41" t="s">
         <v>464</v>
       </c>
@@ -15173,14 +15222,14 @@
       <c r="K14" s="43" t="s">
         <v>530</v>
       </c>
-      <c r="L14" s="112"/>
-      <c r="M14" s="112"/>
+      <c r="L14" s="111"/>
+      <c r="M14" s="111"/>
     </row>
     <row r="15" spans="1:13" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A15" s="100"/>
-      <c r="B15" s="100"/>
-      <c r="C15" s="100"/>
-      <c r="D15" s="115"/>
+      <c r="A15" s="103"/>
+      <c r="B15" s="103"/>
+      <c r="C15" s="103"/>
+      <c r="D15" s="107"/>
       <c r="E15" s="41" t="s">
         <v>465</v>
       </c>
@@ -15200,56 +15249,56 @@
       <c r="K15" s="43" t="s">
         <v>534</v>
       </c>
-      <c r="L15" s="112"/>
-      <c r="M15" s="112"/>
+      <c r="L15" s="111"/>
+      <c r="M15" s="111"/>
     </row>
     <row r="16" spans="1:13" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A16" s="100"/>
-      <c r="B16" s="100"/>
-      <c r="C16" s="100"/>
-      <c r="D16" s="115"/>
-      <c r="E16" s="99" t="s">
+      <c r="A16" s="103"/>
+      <c r="B16" s="103"/>
+      <c r="C16" s="103"/>
+      <c r="D16" s="107"/>
+      <c r="E16" s="102" t="s">
         <v>467</v>
       </c>
-      <c r="F16" s="102" t="s">
+      <c r="F16" s="113" t="s">
         <v>535</v>
       </c>
       <c r="G16" s="78"/>
-      <c r="H16" s="123"/>
+      <c r="H16" s="122"/>
       <c r="I16" s="63" t="s">
         <v>536</v>
       </c>
       <c r="J16" s="46"/>
       <c r="K16" s="43"/>
-      <c r="L16" s="112"/>
-      <c r="M16" s="112"/>
+      <c r="L16" s="111"/>
+      <c r="M16" s="111"/>
     </row>
     <row r="17" spans="1:14" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A17" s="100"/>
-      <c r="B17" s="100"/>
-      <c r="C17" s="100"/>
-      <c r="D17" s="115"/>
-      <c r="E17" s="100"/>
-      <c r="F17" s="103"/>
+      <c r="A17" s="103"/>
+      <c r="B17" s="103"/>
+      <c r="C17" s="103"/>
+      <c r="D17" s="107"/>
+      <c r="E17" s="103"/>
+      <c r="F17" s="114"/>
       <c r="G17" s="79"/>
-      <c r="H17" s="123"/>
+      <c r="H17" s="122"/>
       <c r="I17" s="63" t="s">
         <v>537</v>
       </c>
       <c r="J17" s="46"/>
       <c r="K17" s="43"/>
-      <c r="L17" s="112"/>
-      <c r="M17" s="112"/>
+      <c r="L17" s="111"/>
+      <c r="M17" s="111"/>
     </row>
     <row r="18" spans="1:14" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A18" s="100"/>
-      <c r="B18" s="100"/>
-      <c r="C18" s="100"/>
-      <c r="D18" s="115"/>
-      <c r="E18" s="100"/>
-      <c r="F18" s="103"/>
+      <c r="A18" s="103"/>
+      <c r="B18" s="103"/>
+      <c r="C18" s="103"/>
+      <c r="D18" s="107"/>
+      <c r="E18" s="103"/>
+      <c r="F18" s="114"/>
       <c r="G18" s="79"/>
-      <c r="H18" s="123"/>
+      <c r="H18" s="122"/>
       <c r="I18" s="43" t="s">
         <v>538</v>
       </c>
@@ -15257,18 +15306,18 @@
       <c r="K18" s="63" t="s">
         <v>539</v>
       </c>
-      <c r="L18" s="112"/>
-      <c r="M18" s="112"/>
+      <c r="L18" s="111"/>
+      <c r="M18" s="111"/>
     </row>
     <row r="19" spans="1:14" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A19" s="100"/>
-      <c r="B19" s="100"/>
-      <c r="C19" s="100"/>
-      <c r="D19" s="115"/>
-      <c r="E19" s="100"/>
-      <c r="F19" s="103"/>
+      <c r="A19" s="103"/>
+      <c r="B19" s="103"/>
+      <c r="C19" s="103"/>
+      <c r="D19" s="107"/>
+      <c r="E19" s="103"/>
+      <c r="F19" s="114"/>
       <c r="G19" s="79"/>
-      <c r="H19" s="123"/>
+      <c r="H19" s="122"/>
       <c r="I19" s="43" t="s">
         <v>540</v>
       </c>
@@ -15276,18 +15325,18 @@
       <c r="K19" s="63" t="s">
         <v>541</v>
       </c>
-      <c r="L19" s="112"/>
-      <c r="M19" s="112"/>
+      <c r="L19" s="111"/>
+      <c r="M19" s="111"/>
     </row>
     <row r="20" spans="1:14" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A20" s="100"/>
-      <c r="B20" s="100"/>
-      <c r="C20" s="100"/>
-      <c r="D20" s="115"/>
-      <c r="E20" s="100"/>
-      <c r="F20" s="103"/>
+      <c r="A20" s="103"/>
+      <c r="B20" s="103"/>
+      <c r="C20" s="103"/>
+      <c r="D20" s="107"/>
+      <c r="E20" s="103"/>
+      <c r="F20" s="114"/>
       <c r="G20" s="79"/>
-      <c r="H20" s="123"/>
+      <c r="H20" s="122"/>
       <c r="I20" s="43" t="s">
         <v>542</v>
       </c>
@@ -15295,44 +15344,44 @@
       <c r="K20" s="63" t="s">
         <v>543</v>
       </c>
-      <c r="L20" s="112"/>
-      <c r="M20" s="112"/>
+      <c r="L20" s="111"/>
+      <c r="M20" s="111"/>
     </row>
     <row r="21" spans="1:14" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A21" s="100"/>
-      <c r="B21" s="100"/>
-      <c r="C21" s="100"/>
-      <c r="D21" s="115"/>
-      <c r="E21" s="100"/>
-      <c r="F21" s="103"/>
+      <c r="A21" s="103"/>
+      <c r="B21" s="103"/>
+      <c r="C21" s="103"/>
+      <c r="D21" s="107"/>
+      <c r="E21" s="103"/>
+      <c r="F21" s="114"/>
       <c r="G21" s="79"/>
-      <c r="H21" s="123"/>
+      <c r="H21" s="122"/>
       <c r="I21" s="45" t="s">
         <v>484</v>
       </c>
       <c r="J21" s="46"/>
       <c r="K21" s="63"/>
-      <c r="L21" s="112"/>
-      <c r="M21" s="112"/>
+      <c r="L21" s="111"/>
+      <c r="M21" s="111"/>
     </row>
     <row r="22" spans="1:14" s="18" customFormat="1" ht="23" customHeight="1">
-      <c r="A22" s="101"/>
-      <c r="B22" s="101"/>
-      <c r="C22" s="101"/>
-      <c r="D22" s="116"/>
-      <c r="E22" s="101"/>
-      <c r="F22" s="104"/>
+      <c r="A22" s="104"/>
+      <c r="B22" s="104"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="109"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="115"/>
       <c r="G22" s="58" t="s">
         <v>582</v>
       </c>
-      <c r="H22" s="123"/>
+      <c r="H22" s="122"/>
       <c r="I22" s="43" t="s">
         <v>544</v>
       </c>
       <c r="J22" s="46"/>
       <c r="K22" s="44"/>
-      <c r="L22" s="113"/>
-      <c r="M22" s="113"/>
+      <c r="L22" s="112"/>
+      <c r="M22" s="112"/>
     </row>
     <row r="23" spans="1:14" s="18" customFormat="1" ht="8" customHeight="1">
       <c r="A23" s="64"/>
@@ -15350,26 +15399,26 @@
       <c r="M23" s="69"/>
     </row>
     <row r="24" spans="1:14" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A24" s="99" t="s">
+      <c r="A24" s="102" t="s">
         <v>468</v>
       </c>
-      <c r="B24" s="117" t="s">
+      <c r="B24" s="123" t="s">
         <v>469</v>
       </c>
-      <c r="C24" s="99" t="s">
+      <c r="C24" s="102" t="s">
         <v>470</v>
       </c>
-      <c r="D24" s="114" t="s">
+      <c r="D24" s="106" t="s">
         <v>545</v>
       </c>
-      <c r="E24" s="99" t="s">
+      <c r="E24" s="102" t="s">
         <v>471</v>
       </c>
-      <c r="F24" s="102" t="s">
+      <c r="F24" s="113" t="s">
         <v>546</v>
       </c>
       <c r="G24" s="78"/>
-      <c r="H24" s="105" t="s">
+      <c r="H24" s="116" t="s">
         <v>547</v>
       </c>
       <c r="I24" s="44" t="s">
@@ -15381,47 +15430,47 @@
       <c r="K24" s="43" t="s">
         <v>548</v>
       </c>
-      <c r="L24" s="111" t="s">
+      <c r="L24" s="110" t="s">
         <v>507</v>
       </c>
-      <c r="M24" s="98" t="s">
+      <c r="M24" s="120" t="s">
         <v>474</v>
       </c>
       <c r="N24" s="47"/>
     </row>
     <row r="25" spans="1:14" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A25" s="100"/>
-      <c r="B25" s="118"/>
-      <c r="C25" s="100"/>
-      <c r="D25" s="115"/>
-      <c r="E25" s="101"/>
-      <c r="F25" s="104"/>
+      <c r="A25" s="103"/>
+      <c r="B25" s="124"/>
+      <c r="C25" s="103"/>
+      <c r="D25" s="107"/>
+      <c r="E25" s="104"/>
+      <c r="F25" s="115"/>
       <c r="G25" s="58" t="s">
         <v>582</v>
       </c>
-      <c r="H25" s="107"/>
+      <c r="H25" s="118"/>
       <c r="I25" s="44" t="s">
         <v>549</v>
       </c>
       <c r="J25" s="45"/>
       <c r="K25" s="43"/>
-      <c r="L25" s="112"/>
-      <c r="M25" s="98"/>
+      <c r="L25" s="111"/>
+      <c r="M25" s="120"/>
       <c r="N25" s="47"/>
     </row>
     <row r="26" spans="1:14" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A26" s="100"/>
-      <c r="B26" s="118"/>
-      <c r="C26" s="100"/>
-      <c r="D26" s="115"/>
-      <c r="E26" s="99" t="s">
+      <c r="A26" s="103"/>
+      <c r="B26" s="124"/>
+      <c r="C26" s="103"/>
+      <c r="D26" s="107"/>
+      <c r="E26" s="102" t="s">
         <v>475</v>
       </c>
-      <c r="F26" s="102" t="s">
+      <c r="F26" s="113" t="s">
         <v>550</v>
       </c>
       <c r="G26" s="78"/>
-      <c r="H26" s="105" t="s">
+      <c r="H26" s="116" t="s">
         <v>551</v>
       </c>
       <c r="I26" s="44" t="s">
@@ -15433,21 +15482,21 @@
       <c r="K26" s="43" t="s">
         <v>553</v>
       </c>
-      <c r="L26" s="112"/>
-      <c r="M26" s="98"/>
+      <c r="L26" s="111"/>
+      <c r="M26" s="120"/>
       <c r="N26" s="47"/>
     </row>
     <row r="27" spans="1:14" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A27" s="100"/>
-      <c r="B27" s="118"/>
-      <c r="C27" s="100"/>
-      <c r="D27" s="115"/>
-      <c r="E27" s="101"/>
-      <c r="F27" s="104"/>
+      <c r="A27" s="103"/>
+      <c r="B27" s="124"/>
+      <c r="C27" s="103"/>
+      <c r="D27" s="107"/>
+      <c r="E27" s="104"/>
+      <c r="F27" s="115"/>
       <c r="G27" s="58" t="s">
         <v>583</v>
       </c>
-      <c r="H27" s="107"/>
+      <c r="H27" s="118"/>
       <c r="I27" s="44" t="s">
         <v>483</v>
       </c>
@@ -15455,15 +15504,15 @@
         <v>479</v>
       </c>
       <c r="K27" s="43"/>
-      <c r="L27" s="112"/>
-      <c r="M27" s="98"/>
+      <c r="L27" s="111"/>
+      <c r="M27" s="120"/>
       <c r="N27" s="47"/>
     </row>
     <row r="28" spans="1:14" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A28" s="100"/>
-      <c r="B28" s="118"/>
-      <c r="C28" s="100"/>
-      <c r="D28" s="115"/>
+      <c r="A28" s="103"/>
+      <c r="B28" s="124"/>
+      <c r="C28" s="103"/>
+      <c r="D28" s="107"/>
       <c r="E28" s="41" t="s">
         <v>477</v>
       </c>
@@ -15482,15 +15531,15 @@
       <c r="K28" s="43" t="s">
         <v>556</v>
       </c>
-      <c r="L28" s="112"/>
-      <c r="M28" s="98"/>
+      <c r="L28" s="111"/>
+      <c r="M28" s="120"/>
       <c r="N28" s="47"/>
     </row>
     <row r="29" spans="1:14" s="18" customFormat="1" ht="19" customHeight="1">
-      <c r="A29" s="101"/>
-      <c r="B29" s="119"/>
-      <c r="C29" s="101"/>
-      <c r="D29" s="116"/>
+      <c r="A29" s="104"/>
+      <c r="B29" s="125"/>
+      <c r="C29" s="104"/>
+      <c r="D29" s="109"/>
       <c r="E29" s="41" t="s">
         <v>480</v>
       </c>
@@ -15512,8 +15561,8 @@
       <c r="K29" s="43" t="s">
         <v>559</v>
       </c>
-      <c r="L29" s="113"/>
-      <c r="M29" s="98"/>
+      <c r="L29" s="112"/>
+      <c r="M29" s="120"/>
       <c r="N29" s="47"/>
     </row>
     <row r="30" spans="1:14" s="18" customFormat="1" ht="8" customHeight="1">
@@ -15532,26 +15581,26 @@
       <c r="M30" s="69"/>
     </row>
     <row r="31" spans="1:14" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A31" s="99" t="s">
+      <c r="A31" s="102" t="s">
         <v>485</v>
       </c>
-      <c r="B31" s="99" t="s">
+      <c r="B31" s="102" t="s">
         <v>486</v>
       </c>
-      <c r="C31" s="99" t="s">
+      <c r="C31" s="102" t="s">
         <v>487</v>
       </c>
-      <c r="D31" s="114" t="s">
+      <c r="D31" s="106" t="s">
         <v>560</v>
       </c>
-      <c r="E31" s="99" t="s">
+      <c r="E31" s="102" t="s">
         <v>488</v>
       </c>
-      <c r="F31" s="102" t="s">
+      <c r="F31" s="113" t="s">
         <v>561</v>
       </c>
       <c r="G31" s="78"/>
-      <c r="H31" s="105" t="s">
+      <c r="H31" s="116" t="s">
         <v>562</v>
       </c>
       <c r="I31" s="76" t="s">
@@ -15563,22 +15612,22 @@
       <c r="K31" s="43" t="s">
         <v>564</v>
       </c>
-      <c r="L31" s="98" t="s">
+      <c r="L31" s="120" t="s">
         <v>490</v>
       </c>
-      <c r="M31" s="98" t="s">
+      <c r="M31" s="120" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="32" spans="1:14" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A32" s="100"/>
-      <c r="B32" s="100"/>
-      <c r="C32" s="100"/>
-      <c r="D32" s="115"/>
-      <c r="E32" s="100"/>
-      <c r="F32" s="103"/>
+      <c r="A32" s="103"/>
+      <c r="B32" s="103"/>
+      <c r="C32" s="103"/>
+      <c r="D32" s="107"/>
+      <c r="E32" s="103"/>
+      <c r="F32" s="114"/>
       <c r="G32" s="79"/>
-      <c r="H32" s="106"/>
+      <c r="H32" s="117"/>
       <c r="I32" s="51" t="s">
         <v>565</v>
       </c>
@@ -15586,79 +15635,79 @@
       <c r="K32" s="43" t="s">
         <v>566</v>
       </c>
-      <c r="L32" s="98"/>
-      <c r="M32" s="98"/>
+      <c r="L32" s="120"/>
+      <c r="M32" s="120"/>
     </row>
     <row r="33" spans="1:13" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A33" s="100"/>
-      <c r="B33" s="100"/>
-      <c r="C33" s="100"/>
-      <c r="D33" s="115"/>
-      <c r="E33" s="101"/>
-      <c r="F33" s="104"/>
+      <c r="A33" s="103"/>
+      <c r="B33" s="103"/>
+      <c r="C33" s="103"/>
+      <c r="D33" s="107"/>
+      <c r="E33" s="104"/>
+      <c r="F33" s="115"/>
       <c r="G33" s="58" t="s">
         <v>582</v>
       </c>
-      <c r="H33" s="107"/>
+      <c r="H33" s="118"/>
       <c r="I33" s="51" t="s">
         <v>500</v>
       </c>
       <c r="J33" s="44"/>
       <c r="K33" s="43"/>
-      <c r="L33" s="98"/>
-      <c r="M33" s="98"/>
+      <c r="L33" s="120"/>
+      <c r="M33" s="120"/>
     </row>
     <row r="34" spans="1:13" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A34" s="100"/>
-      <c r="B34" s="100"/>
-      <c r="C34" s="100"/>
-      <c r="D34" s="115"/>
-      <c r="E34" s="99" t="s">
+      <c r="A34" s="103"/>
+      <c r="B34" s="103"/>
+      <c r="C34" s="103"/>
+      <c r="D34" s="107"/>
+      <c r="E34" s="102" t="s">
         <v>492</v>
       </c>
-      <c r="F34" s="102" t="s">
+      <c r="F34" s="113" t="s">
         <v>567</v>
       </c>
       <c r="G34" s="78"/>
-      <c r="H34" s="105" t="s">
+      <c r="H34" s="116" t="s">
         <v>568</v>
       </c>
       <c r="I34" s="44" t="s">
         <v>569</v>
       </c>
       <c r="J34" s="44"/>
-      <c r="K34" s="108"/>
-      <c r="L34" s="98"/>
-      <c r="M34" s="98"/>
+      <c r="K34" s="126"/>
+      <c r="L34" s="120"/>
+      <c r="M34" s="120"/>
     </row>
     <row r="35" spans="1:13" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A35" s="100"/>
-      <c r="B35" s="100"/>
-      <c r="C35" s="100"/>
-      <c r="D35" s="115"/>
-      <c r="E35" s="100"/>
-      <c r="F35" s="103"/>
+      <c r="A35" s="103"/>
+      <c r="B35" s="103"/>
+      <c r="C35" s="103"/>
+      <c r="D35" s="107"/>
+      <c r="E35" s="103"/>
+      <c r="F35" s="114"/>
       <c r="G35" s="79"/>
-      <c r="H35" s="106"/>
+      <c r="H35" s="117"/>
       <c r="I35" s="44" t="s">
         <v>496</v>
       </c>
       <c r="J35" s="44"/>
-      <c r="K35" s="108"/>
-      <c r="L35" s="98"/>
-      <c r="M35" s="98"/>
+      <c r="K35" s="126"/>
+      <c r="L35" s="120"/>
+      <c r="M35" s="120"/>
     </row>
     <row r="36" spans="1:13" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A36" s="100"/>
-      <c r="B36" s="100"/>
-      <c r="C36" s="100"/>
-      <c r="D36" s="115"/>
-      <c r="E36" s="101"/>
-      <c r="F36" s="104"/>
+      <c r="A36" s="103"/>
+      <c r="B36" s="103"/>
+      <c r="C36" s="103"/>
+      <c r="D36" s="107"/>
+      <c r="E36" s="104"/>
+      <c r="F36" s="115"/>
       <c r="G36" s="58" t="s">
         <v>582</v>
       </c>
-      <c r="H36" s="107"/>
+      <c r="H36" s="118"/>
       <c r="I36" s="44" t="s">
         <v>570</v>
       </c>
@@ -15668,68 +15717,68 @@
       <c r="K36" s="43" t="s">
         <v>494</v>
       </c>
-      <c r="L36" s="98"/>
-      <c r="M36" s="98"/>
+      <c r="L36" s="120"/>
+      <c r="M36" s="120"/>
     </row>
     <row r="37" spans="1:13" s="18" customFormat="1" ht="18" customHeight="1">
-      <c r="A37" s="100"/>
-      <c r="B37" s="100"/>
-      <c r="C37" s="100"/>
-      <c r="D37" s="115"/>
-      <c r="E37" s="99" t="s">
+      <c r="A37" s="103"/>
+      <c r="B37" s="103"/>
+      <c r="C37" s="103"/>
+      <c r="D37" s="107"/>
+      <c r="E37" s="102" t="s">
         <v>495</v>
       </c>
-      <c r="F37" s="102" t="s">
+      <c r="F37" s="113" t="s">
         <v>571</v>
       </c>
       <c r="G37" s="78"/>
-      <c r="H37" s="109" t="s">
+      <c r="H37" s="127" t="s">
         <v>572</v>
       </c>
       <c r="I37" s="44" t="s">
         <v>573</v>
       </c>
-      <c r="J37" s="110" t="s">
+      <c r="J37" s="128" t="s">
         <v>497</v>
       </c>
-      <c r="K37" s="109" t="s">
+      <c r="K37" s="127" t="s">
         <v>499</v>
       </c>
-      <c r="L37" s="98"/>
-      <c r="M37" s="98"/>
+      <c r="L37" s="120"/>
+      <c r="M37" s="120"/>
     </row>
     <row r="38" spans="1:13" s="18" customFormat="1" ht="18" customHeight="1">
-      <c r="A38" s="100"/>
-      <c r="B38" s="100"/>
-      <c r="C38" s="100"/>
-      <c r="D38" s="115"/>
-      <c r="E38" s="100"/>
-      <c r="F38" s="103"/>
+      <c r="A38" s="103"/>
+      <c r="B38" s="103"/>
+      <c r="C38" s="103"/>
+      <c r="D38" s="107"/>
+      <c r="E38" s="103"/>
+      <c r="F38" s="114"/>
       <c r="G38" s="79" t="s">
         <v>582</v>
       </c>
-      <c r="H38" s="109"/>
+      <c r="H38" s="127"/>
       <c r="I38" s="63" t="s">
         <v>574</v>
       </c>
-      <c r="J38" s="110"/>
-      <c r="K38" s="109"/>
-      <c r="L38" s="98"/>
-      <c r="M38" s="98"/>
+      <c r="J38" s="128"/>
+      <c r="K38" s="127"/>
+      <c r="L38" s="120"/>
+      <c r="M38" s="120"/>
     </row>
     <row r="39" spans="1:13" s="18" customFormat="1" ht="18" customHeight="1">
-      <c r="A39" s="100"/>
-      <c r="B39" s="100"/>
-      <c r="C39" s="100"/>
-      <c r="D39" s="115"/>
-      <c r="E39" s="100" t="s">
+      <c r="A39" s="103"/>
+      <c r="B39" s="103"/>
+      <c r="C39" s="103"/>
+      <c r="D39" s="107"/>
+      <c r="E39" s="103" t="s">
         <v>498</v>
       </c>
-      <c r="F39" s="103" t="s">
+      <c r="F39" s="114" t="s">
         <v>575</v>
       </c>
       <c r="G39" s="79"/>
-      <c r="H39" s="109" t="s">
+      <c r="H39" s="127" t="s">
         <v>576</v>
       </c>
       <c r="I39" s="63" t="s">
@@ -15739,18 +15788,18 @@
       <c r="K39" s="51" t="s">
         <v>578</v>
       </c>
-      <c r="L39" s="98"/>
-      <c r="M39" s="98"/>
+      <c r="L39" s="120"/>
+      <c r="M39" s="120"/>
     </row>
     <row r="40" spans="1:13" s="18" customFormat="1" ht="18" customHeight="1">
-      <c r="A40" s="100"/>
-      <c r="B40" s="100"/>
-      <c r="C40" s="100"/>
-      <c r="D40" s="115"/>
-      <c r="E40" s="100"/>
-      <c r="F40" s="103"/>
+      <c r="A40" s="103"/>
+      <c r="B40" s="103"/>
+      <c r="C40" s="103"/>
+      <c r="D40" s="107"/>
+      <c r="E40" s="103"/>
+      <c r="F40" s="114"/>
       <c r="G40" s="79"/>
-      <c r="H40" s="109"/>
+      <c r="H40" s="127"/>
       <c r="I40" s="63" t="s">
         <v>579</v>
       </c>
@@ -15758,27 +15807,27 @@
       <c r="K40" s="51" t="s">
         <v>580</v>
       </c>
-      <c r="L40" s="98"/>
-      <c r="M40" s="98"/>
+      <c r="L40" s="120"/>
+      <c r="M40" s="120"/>
     </row>
     <row r="41" spans="1:13" s="18" customFormat="1" ht="17" customHeight="1">
-      <c r="A41" s="101"/>
-      <c r="B41" s="101"/>
-      <c r="C41" s="101"/>
-      <c r="D41" s="116"/>
-      <c r="E41" s="101"/>
-      <c r="F41" s="104"/>
+      <c r="A41" s="104"/>
+      <c r="B41" s="104"/>
+      <c r="C41" s="104"/>
+      <c r="D41" s="109"/>
+      <c r="E41" s="104"/>
+      <c r="F41" s="115"/>
       <c r="G41" s="58" t="s">
         <v>582</v>
       </c>
-      <c r="H41" s="109"/>
+      <c r="H41" s="127"/>
       <c r="I41" s="63" t="s">
         <v>581</v>
       </c>
       <c r="J41" s="46"/>
       <c r="K41" s="43"/>
-      <c r="L41" s="98"/>
-      <c r="M41" s="98"/>
+      <c r="L41" s="120"/>
+      <c r="M41" s="120"/>
     </row>
     <row r="42" spans="1:13">
       <c r="K42" s="77"/>
@@ -15786,42 +15835,6 @@
     <row r="43" spans="1:13" ht="23" customHeight="1"/>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F4"/>
-    <mergeCell ref="A6:A22"/>
-    <mergeCell ref="B6:B22"/>
-    <mergeCell ref="C6:C12"/>
-    <mergeCell ref="D6:D12"/>
-    <mergeCell ref="C13:C22"/>
-    <mergeCell ref="D13:D22"/>
-    <mergeCell ref="L6:L22"/>
-    <mergeCell ref="M6:M22"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="E16:E22"/>
-    <mergeCell ref="F16:F22"/>
-    <mergeCell ref="H16:H22"/>
-    <mergeCell ref="A24:A29"/>
-    <mergeCell ref="B24:B29"/>
-    <mergeCell ref="C24:C29"/>
-    <mergeCell ref="D24:D29"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="A31:A41"/>
-    <mergeCell ref="B31:B41"/>
-    <mergeCell ref="C31:C41"/>
-    <mergeCell ref="D31:D41"/>
-    <mergeCell ref="E31:E33"/>
-    <mergeCell ref="L24:L29"/>
-    <mergeCell ref="M24:M29"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="H24:H25"/>
     <mergeCell ref="L31:L41"/>
     <mergeCell ref="M31:M41"/>
     <mergeCell ref="E34:E36"/>
@@ -15838,6 +15851,42 @@
     <mergeCell ref="H39:H41"/>
     <mergeCell ref="F31:F33"/>
     <mergeCell ref="H31:H33"/>
+    <mergeCell ref="L24:L29"/>
+    <mergeCell ref="M24:M29"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="A31:A41"/>
+    <mergeCell ref="B31:B41"/>
+    <mergeCell ref="C31:C41"/>
+    <mergeCell ref="D31:D41"/>
+    <mergeCell ref="E31:E33"/>
+    <mergeCell ref="A24:A29"/>
+    <mergeCell ref="B24:B29"/>
+    <mergeCell ref="C24:C29"/>
+    <mergeCell ref="D24:D29"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="L6:L22"/>
+    <mergeCell ref="M6:M22"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="E16:E22"/>
+    <mergeCell ref="F16:F22"/>
+    <mergeCell ref="H16:H22"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F4"/>
+    <mergeCell ref="A6:A22"/>
+    <mergeCell ref="B6:B22"/>
+    <mergeCell ref="C6:C12"/>
+    <mergeCell ref="D6:D12"/>
+    <mergeCell ref="C13:C22"/>
+    <mergeCell ref="D13:D22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H6" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>

</xml_diff>

<commit_message>
notes update post found lab 3
</commit_message>
<xml_diff>
--- a/blueprints-combined.xlsx
+++ b/blueprints-combined.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qdd/Sync/git/notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF91E2CC-076F-D149-AC15-5C6CB4DB8A9C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD25DCB3-3639-A444-9830-F4C5190415B9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39820" yWindow="1040" windowWidth="32840" windowHeight="20520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3760" yWindow="660" windowWidth="30400" windowHeight="20040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lab-topics" sheetId="6" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1775" uniqueCount="963">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1927" uniqueCount="973">
   <si>
     <t>date</t>
   </si>
@@ -2979,9 +2979,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>LAB</t>
-  </si>
-  <si>
     <t>target</t>
   </si>
   <si>
@@ -2997,9 +2994,6 @@
     <t>foundation lab 2</t>
   </si>
   <si>
-    <t>suppress, unsuppress maps</t>
-  </si>
-  <si>
     <t>vrfs not assoc with physical int</t>
   </si>
   <si>
@@ -3010,6 +3004,42 @@
   </si>
   <si>
     <t>ospf domain-id, down bit</t>
+  </si>
+  <si>
+    <t>configure, flash card</t>
+  </si>
+  <si>
+    <t>why disable?</t>
+  </si>
+  <si>
+    <t>conditional debug</t>
+  </si>
+  <si>
+    <t>what are additional extended options</t>
+  </si>
+  <si>
+    <t>practice on ios and iosvl2</t>
+  </si>
+  <si>
+    <t>practice setup, problems</t>
+  </si>
+  <si>
+    <t>more practice</t>
+  </si>
+  <si>
+    <t>internal router</t>
+  </si>
+  <si>
+    <t>suppress, unsuppress maps, as-set</t>
+  </si>
+  <si>
+    <t>glbp</t>
+  </si>
+  <si>
+    <t>udp jitter lab</t>
+  </si>
+  <si>
+    <t>LLDP</t>
   </si>
 </sst>
 </file>
@@ -3182,7 +3212,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3222,12 +3252,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3382,7 +3406,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -3611,8 +3635,13 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3622,6 +3651,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3642,32 +3695,17 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3678,29 +3716,14 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -4184,10 +4207,10 @@
   <dimension ref="A1:Q349"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C157" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A189" sqref="A189"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -4212,7 +4235,7 @@
       </c>
       <c r="G1" s="90">
         <f ca="1">(TODAY()-I1)*-1</f>
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H1" s="91" t="s">
         <v>10</v>
@@ -4232,10 +4255,10 @@
         <v>585</v>
       </c>
       <c r="D2" s="95" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="E2" s="95" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="F2" s="95"/>
       <c r="G2" s="95"/>
@@ -4316,6 +4339,15 @@
       <c r="B10" s="7" t="s">
         <v>606</v>
       </c>
+      <c r="C10" t="s">
+        <v>951</v>
+      </c>
+      <c r="D10" t="s">
+        <v>961</v>
+      </c>
+      <c r="E10" t="s">
+        <v>972</v>
+      </c>
     </row>
     <row r="11" spans="1:17" ht="16">
       <c r="A11" s="83" t="s">
@@ -4324,6 +4356,12 @@
       <c r="B11" s="7" t="s">
         <v>607</v>
       </c>
+      <c r="C11" t="s">
+        <v>951</v>
+      </c>
+      <c r="D11" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="12" spans="1:17" ht="16">
       <c r="A12" s="83" t="s">
@@ -4365,7 +4403,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="16">
+    <row r="17" spans="1:4" ht="16">
       <c r="A17" s="83" t="s">
         <v>928</v>
       </c>
@@ -4373,7 +4411,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="16">
+    <row r="18" spans="1:4" ht="16">
       <c r="A18" s="83" t="s">
         <v>928</v>
       </c>
@@ -4381,7 +4419,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="16">
+    <row r="19" spans="1:4" ht="16">
       <c r="A19" s="83" t="s">
         <v>928</v>
       </c>
@@ -4389,7 +4427,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="16">
+    <row r="20" spans="1:4" ht="16">
       <c r="A20" s="83" t="s">
         <v>928</v>
       </c>
@@ -4397,7 +4435,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="16">
+    <row r="21" spans="1:4" ht="16">
       <c r="A21" s="83" t="s">
         <v>928</v>
       </c>
@@ -4405,7 +4443,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="16">
+    <row r="22" spans="1:4" ht="16">
       <c r="A22" s="83" t="s">
         <v>928</v>
       </c>
@@ -4413,7 +4451,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="16">
+    <row r="23" spans="1:4" ht="16">
       <c r="A23" s="83" t="s">
         <v>928</v>
       </c>
@@ -4421,7 +4459,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="16">
+    <row r="24" spans="1:4" ht="16">
       <c r="A24" s="83" t="s">
         <v>928</v>
       </c>
@@ -4429,15 +4467,21 @@
         <v>945</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="16">
+    <row r="25" spans="1:4" ht="16">
       <c r="A25" s="83" t="s">
         <v>928</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>946</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="16">
+      <c r="C25" t="s">
+        <v>951</v>
+      </c>
+      <c r="D25" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="16">
       <c r="A26" s="83" t="s">
         <v>928</v>
       </c>
@@ -4445,7 +4489,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="16">
+    <row r="27" spans="1:4" ht="16">
       <c r="A27" s="83" t="s">
         <v>928</v>
       </c>
@@ -4453,7 +4497,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="16">
+    <row r="28" spans="1:4" ht="16">
       <c r="A28" s="83" t="s">
         <v>928</v>
       </c>
@@ -4461,7 +4505,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="16">
+    <row r="29" spans="1:4" ht="16">
       <c r="A29" s="83" t="s">
         <v>928</v>
       </c>
@@ -4469,7 +4513,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="16">
+    <row r="30" spans="1:4" ht="16">
       <c r="A30" s="83" t="s">
         <v>928</v>
       </c>
@@ -4477,7 +4521,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="16">
+    <row r="31" spans="1:4" ht="16">
       <c r="A31" s="83" t="s">
         <v>928</v>
       </c>
@@ -4485,12 +4529,18 @@
         <v>620</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="16">
+    <row r="32" spans="1:4" ht="16">
       <c r="A32" s="83" t="s">
         <v>928</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>621</v>
+      </c>
+      <c r="C32" t="s">
+        <v>951</v>
+      </c>
+      <c r="D32" t="s">
+        <v>961</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="19">
@@ -4541,8 +4591,9 @@
       <c r="B37" s="7" t="s">
         <v>626</v>
       </c>
-      <c r="C37" s="98"/>
-      <c r="D37" s="98"/>
+      <c r="C37" t="s">
+        <v>951</v>
+      </c>
     </row>
     <row r="38" spans="1:4" ht="16">
       <c r="A38" s="83" t="s">
@@ -4551,8 +4602,9 @@
       <c r="B38" s="7" t="s">
         <v>627</v>
       </c>
-      <c r="C38" s="98"/>
-      <c r="D38" s="98"/>
+      <c r="C38" t="s">
+        <v>951</v>
+      </c>
     </row>
     <row r="39" spans="1:4" ht="16">
       <c r="A39" s="83" t="s">
@@ -4561,8 +4613,9 @@
       <c r="B39" s="7" t="s">
         <v>628</v>
       </c>
-      <c r="C39" s="98"/>
-      <c r="D39" s="98"/>
+      <c r="C39" t="s">
+        <v>951</v>
+      </c>
     </row>
     <row r="40" spans="1:4" ht="19">
       <c r="A40" s="83" t="s">
@@ -4603,9 +4656,6 @@
       <c r="B44" s="7" t="s">
         <v>633</v>
       </c>
-      <c r="C44" t="s">
-        <v>952</v>
-      </c>
     </row>
     <row r="45" spans="1:4" ht="16">
       <c r="A45" s="83" t="s">
@@ -4615,7 +4665,10 @@
         <v>634</v>
       </c>
       <c r="C45" t="s">
-        <v>952</v>
+        <v>951</v>
+      </c>
+      <c r="D45" t="s">
+        <v>961</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="19">
@@ -4641,6 +4694,12 @@
       <c r="B48" s="88" t="s">
         <v>637</v>
       </c>
+      <c r="C48" t="s">
+        <v>951</v>
+      </c>
+      <c r="D48" t="s">
+        <v>963</v>
+      </c>
     </row>
     <row r="49" spans="1:5" ht="16">
       <c r="A49" s="83" t="s">
@@ -4649,6 +4708,12 @@
       <c r="B49" s="88" t="s">
         <v>638</v>
       </c>
+      <c r="C49" t="s">
+        <v>951</v>
+      </c>
+      <c r="D49" t="s">
+        <v>964</v>
+      </c>
     </row>
     <row r="50" spans="1:5" ht="16">
       <c r="A50" s="83" t="s">
@@ -4656,6 +4721,12 @@
       </c>
       <c r="B50" s="88" t="s">
         <v>639</v>
+      </c>
+      <c r="C50" t="s">
+        <v>951</v>
+      </c>
+      <c r="D50" t="s">
+        <v>965</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="16">
@@ -4740,9 +4811,6 @@
       <c r="B60" s="7" t="s">
         <v>650</v>
       </c>
-      <c r="C60" t="s">
-        <v>951</v>
-      </c>
     </row>
     <row r="61" spans="1:5" ht="16">
       <c r="A61" s="83" t="s">
@@ -4751,9 +4819,6 @@
       <c r="B61" s="7" t="s">
         <v>651</v>
       </c>
-      <c r="C61" t="s">
-        <v>951</v>
-      </c>
     </row>
     <row r="62" spans="1:5" ht="16">
       <c r="A62" s="83" t="s">
@@ -4762,9 +4827,6 @@
       <c r="B62" s="7" t="s">
         <v>652</v>
       </c>
-      <c r="C62" t="s">
-        <v>951</v>
-      </c>
     </row>
     <row r="63" spans="1:5" ht="16">
       <c r="A63" s="83" t="s">
@@ -4776,6 +4838,9 @@
       <c r="C63" t="s">
         <v>951</v>
       </c>
+      <c r="D63" t="s">
+        <v>966</v>
+      </c>
     </row>
     <row r="64" spans="1:5" ht="16">
       <c r="A64" s="83" t="s">
@@ -4784,9 +4849,6 @@
       <c r="B64" s="7" t="s">
         <v>654</v>
       </c>
-      <c r="C64" t="s">
-        <v>951</v>
-      </c>
     </row>
     <row r="65" spans="1:5" ht="16">
       <c r="A65" s="83" t="s">
@@ -4798,6 +4860,9 @@
       <c r="C65" t="s">
         <v>951</v>
       </c>
+      <c r="D65" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="66" spans="1:5" ht="16">
       <c r="A66" s="83" t="s">
@@ -4809,6 +4874,9 @@
       <c r="C66" t="s">
         <v>951</v>
       </c>
+      <c r="D66" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="67" spans="1:5" ht="16">
       <c r="A67" s="83" t="s">
@@ -4820,6 +4888,9 @@
       <c r="C67" t="s">
         <v>951</v>
       </c>
+      <c r="D67" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="68" spans="1:5" ht="16">
       <c r="A68" s="83" t="s">
@@ -4831,6 +4902,9 @@
       <c r="C68" t="s">
         <v>951</v>
       </c>
+      <c r="D68" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="69" spans="1:5" ht="19">
       <c r="A69" s="83" t="s">
@@ -4847,9 +4921,6 @@
       <c r="B70" s="7" t="s">
         <v>659</v>
       </c>
-      <c r="C70" t="s">
-        <v>951</v>
-      </c>
     </row>
     <row r="71" spans="1:5" ht="16">
       <c r="A71" s="83" t="s">
@@ -4858,9 +4929,6 @@
       <c r="B71" s="7" t="s">
         <v>660</v>
       </c>
-      <c r="C71" t="s">
-        <v>951</v>
-      </c>
     </row>
     <row r="72" spans="1:5" ht="16">
       <c r="A72" s="83" t="s">
@@ -4869,9 +4937,6 @@
       <c r="B72" s="7" t="s">
         <v>661</v>
       </c>
-      <c r="C72" t="s">
-        <v>951</v>
-      </c>
     </row>
     <row r="73" spans="1:5" ht="16">
       <c r="A73" s="83" t="s">
@@ -4880,9 +4945,6 @@
       <c r="B73" s="7" t="s">
         <v>662</v>
       </c>
-      <c r="C73" t="s">
-        <v>951</v>
-      </c>
       <c r="E73" s="89" t="s">
         <v>950</v>
       </c>
@@ -4894,9 +4956,6 @@
       <c r="B74" s="7" t="s">
         <v>663</v>
       </c>
-      <c r="C74" t="s">
-        <v>951</v>
-      </c>
     </row>
     <row r="75" spans="1:5" ht="16">
       <c r="A75" s="83" t="s">
@@ -4908,6 +4967,9 @@
       <c r="C75" t="s">
         <v>951</v>
       </c>
+      <c r="D75" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="76" spans="1:5" ht="16">
       <c r="A76" s="83" t="s">
@@ -4919,6 +4981,9 @@
       <c r="C76" t="s">
         <v>951</v>
       </c>
+      <c r="D76" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="77" spans="1:5" ht="16">
       <c r="A77" s="83" t="s">
@@ -4930,6 +4995,9 @@
       <c r="C77" t="s">
         <v>951</v>
       </c>
+      <c r="D77" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="78" spans="1:5" ht="16">
       <c r="A78" s="83" t="s">
@@ -4941,6 +5009,9 @@
       <c r="C78" t="s">
         <v>951</v>
       </c>
+      <c r="D78" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="79" spans="1:5" ht="16">
       <c r="A79" s="83" t="s">
@@ -4952,6 +5023,9 @@
       <c r="C79" t="s">
         <v>951</v>
       </c>
+      <c r="D79" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="80" spans="1:5" ht="16">
       <c r="A80" s="83" t="s">
@@ -4963,6 +5037,9 @@
       <c r="C80" t="s">
         <v>951</v>
       </c>
+      <c r="D80" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="81" spans="1:4" ht="16">
       <c r="A81" s="83" t="s">
@@ -4974,6 +5051,9 @@
       <c r="C81" t="s">
         <v>951</v>
       </c>
+      <c r="D81" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="82" spans="1:4" ht="16">
       <c r="A82" s="83" t="s">
@@ -4982,8 +5062,12 @@
       <c r="B82" s="7" t="s">
         <v>671</v>
       </c>
-      <c r="C82" s="98"/>
-      <c r="D82" s="98"/>
+      <c r="C82" t="s">
+        <v>951</v>
+      </c>
+      <c r="D82" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="83" spans="1:4" ht="19">
       <c r="A83" s="83" t="s">
@@ -5080,6 +5164,12 @@
       <c r="B94" s="7" t="s">
         <v>679</v>
       </c>
+      <c r="C94" t="s">
+        <v>951</v>
+      </c>
+      <c r="D94" t="s">
+        <v>967</v>
+      </c>
     </row>
     <row r="95" spans="1:4" ht="16">
       <c r="A95" s="83" t="s">
@@ -5097,7 +5187,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="16">
+    <row r="97" spans="1:4" ht="16">
       <c r="A97" s="83" t="s">
         <v>929</v>
       </c>
@@ -5105,7 +5195,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="16">
+    <row r="98" spans="1:4" ht="16">
       <c r="A98" s="83" t="s">
         <v>929</v>
       </c>
@@ -5113,7 +5203,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="16">
+    <row r="99" spans="1:4" ht="16">
       <c r="A99" s="83" t="s">
         <v>929</v>
       </c>
@@ -5121,7 +5211,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="16">
+    <row r="100" spans="1:4" ht="16">
       <c r="A100" s="83" t="s">
         <v>929</v>
       </c>
@@ -5129,7 +5219,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="16">
+    <row r="101" spans="1:4" ht="16">
       <c r="A101" s="83" t="s">
         <v>929</v>
       </c>
@@ -5137,7 +5227,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="16">
+    <row r="102" spans="1:4" ht="16">
       <c r="A102" s="83" t="s">
         <v>929</v>
       </c>
@@ -5145,7 +5235,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="16">
+    <row r="103" spans="1:4" ht="16">
       <c r="A103" s="83" t="s">
         <v>929</v>
       </c>
@@ -5153,7 +5243,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="16">
+    <row r="104" spans="1:4" ht="16">
       <c r="A104" s="83" t="s">
         <v>929</v>
       </c>
@@ -5161,7 +5251,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="16">
+    <row r="105" spans="1:4" ht="16">
       <c r="A105" s="83" t="s">
         <v>929</v>
       </c>
@@ -5169,7 +5259,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="16">
+    <row r="106" spans="1:4" ht="16">
       <c r="A106" s="83" t="s">
         <v>929</v>
       </c>
@@ -5177,7 +5267,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="16">
+    <row r="107" spans="1:4" ht="16">
       <c r="A107" s="83" t="s">
         <v>929</v>
       </c>
@@ -5185,15 +5275,21 @@
         <v>692</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="16">
+    <row r="108" spans="1:4" ht="16">
       <c r="A108" s="83" t="s">
         <v>929</v>
       </c>
       <c r="B108" s="7" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" ht="19">
+      <c r="C108" t="s">
+        <v>951</v>
+      </c>
+      <c r="D108" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="19">
       <c r="A109" s="83" t="s">
         <v>929</v>
       </c>
@@ -5201,7 +5297,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="16">
+    <row r="110" spans="1:4" ht="16">
       <c r="A110" s="83" t="s">
         <v>929</v>
       </c>
@@ -5209,7 +5305,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="19">
+    <row r="111" spans="1:4" ht="19">
       <c r="A111" s="83" t="s">
         <v>929</v>
       </c>
@@ -5217,7 +5313,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="16">
+    <row r="112" spans="1:4" ht="16">
       <c r="A112" s="83" t="s">
         <v>929</v>
       </c>
@@ -5225,7 +5321,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="16">
+    <row r="113" spans="1:4" ht="16">
       <c r="A113" s="83" t="s">
         <v>929</v>
       </c>
@@ -5233,7 +5329,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="16">
+    <row r="114" spans="1:4" ht="16">
       <c r="A114" s="83" t="s">
         <v>929</v>
       </c>
@@ -5241,15 +5337,21 @@
         <v>699</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="16">
+    <row r="115" spans="1:4" ht="16">
       <c r="A115" s="83" t="s">
         <v>929</v>
       </c>
       <c r="B115" s="7" t="s">
         <v>700</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" ht="16">
+      <c r="C115" t="s">
+        <v>951</v>
+      </c>
+      <c r="D115" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="16">
       <c r="A116" s="83" t="s">
         <v>929</v>
       </c>
@@ -5257,7 +5359,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="16">
+    <row r="117" spans="1:4" ht="16">
       <c r="A117" s="83" t="s">
         <v>929</v>
       </c>
@@ -5265,7 +5367,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="16">
+    <row r="118" spans="1:4" ht="16">
       <c r="A118" s="83" t="s">
         <v>929</v>
       </c>
@@ -5273,7 +5375,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="16">
+    <row r="119" spans="1:4" ht="16">
       <c r="A119" s="83" t="s">
         <v>929</v>
       </c>
@@ -5281,7 +5383,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="16">
+    <row r="120" spans="1:4" ht="16">
       <c r="A120" s="83" t="s">
         <v>929</v>
       </c>
@@ -5289,7 +5391,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="16">
+    <row r="121" spans="1:4" ht="16">
       <c r="A121" s="83" t="s">
         <v>929</v>
       </c>
@@ -5297,7 +5399,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="16">
+    <row r="122" spans="1:4" ht="16">
       <c r="A122" s="83" t="s">
         <v>929</v>
       </c>
@@ -5305,7 +5407,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="16">
+    <row r="123" spans="1:4" ht="16">
       <c r="A123" s="83" t="s">
         <v>929</v>
       </c>
@@ -5313,7 +5415,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="16">
+    <row r="124" spans="1:4" ht="16">
       <c r="A124" s="83" t="s">
         <v>929</v>
       </c>
@@ -5321,15 +5423,21 @@
         <v>709</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="16">
+    <row r="125" spans="1:4" ht="16">
       <c r="A125" s="83" t="s">
         <v>929</v>
       </c>
       <c r="B125" s="7" t="s">
         <v>710</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" ht="16">
+      <c r="C125" t="s">
+        <v>951</v>
+      </c>
+      <c r="D125" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="16">
       <c r="A126" s="83" t="s">
         <v>929</v>
       </c>
@@ -5337,7 +5445,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="16">
+    <row r="127" spans="1:4" ht="16">
       <c r="A127" s="83" t="s">
         <v>929</v>
       </c>
@@ -5345,7 +5453,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="16">
+    <row r="128" spans="1:4" ht="16">
       <c r="A128" s="83" t="s">
         <v>929</v>
       </c>
@@ -5353,7 +5461,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="16">
+    <row r="129" spans="1:4" ht="16">
       <c r="A129" s="83" t="s">
         <v>929</v>
       </c>
@@ -5361,7 +5469,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="16">
+    <row r="130" spans="1:4" ht="16">
       <c r="A130" s="83" t="s">
         <v>929</v>
       </c>
@@ -5369,7 +5477,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="16">
+    <row r="131" spans="1:4" ht="16">
       <c r="A131" s="83" t="s">
         <v>929</v>
       </c>
@@ -5377,15 +5485,21 @@
         <v>716</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="16">
+    <row r="132" spans="1:4" ht="16">
       <c r="A132" s="83" t="s">
         <v>929</v>
       </c>
       <c r="B132" s="7" t="s">
         <v>717</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" ht="16">
+      <c r="C132" t="s">
+        <v>951</v>
+      </c>
+      <c r="D132" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="16">
       <c r="A133" s="83" t="s">
         <v>929</v>
       </c>
@@ -5393,7 +5507,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="16">
+    <row r="134" spans="1:4" ht="16">
       <c r="A134" s="83" t="s">
         <v>929</v>
       </c>
@@ -5401,7 +5515,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="16">
+    <row r="135" spans="1:4" ht="16">
       <c r="A135" s="83" t="s">
         <v>929</v>
       </c>
@@ -5409,7 +5523,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="16">
+    <row r="136" spans="1:4" ht="16">
       <c r="A136" s="83" t="s">
         <v>929</v>
       </c>
@@ -5420,7 +5534,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="16">
+    <row r="137" spans="1:4" ht="16">
       <c r="A137" s="83" t="s">
         <v>929</v>
       </c>
@@ -5428,7 +5542,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="16">
+    <row r="138" spans="1:4" ht="16">
       <c r="A138" s="83" t="s">
         <v>929</v>
       </c>
@@ -5436,10 +5550,13 @@
         <v>723</v>
       </c>
       <c r="C138" t="s">
-        <v>952</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" ht="16">
+        <v>951</v>
+      </c>
+      <c r="D138" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" ht="16">
       <c r="A139" s="83" t="s">
         <v>929</v>
       </c>
@@ -5447,15 +5564,21 @@
         <v>724</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="16">
+    <row r="140" spans="1:4" ht="16">
       <c r="A140" s="83" t="s">
         <v>929</v>
       </c>
       <c r="B140" s="7" t="s">
         <v>725</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" ht="16">
+      <c r="C140" t="s">
+        <v>951</v>
+      </c>
+      <c r="D140" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="16">
       <c r="A141" s="83" t="s">
         <v>929</v>
       </c>
@@ -5463,7 +5586,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="16">
+    <row r="142" spans="1:4" ht="16">
       <c r="A142" s="83" t="s">
         <v>929</v>
       </c>
@@ -5471,7 +5594,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="19">
+    <row r="143" spans="1:4" ht="19">
       <c r="A143" s="83" t="s">
         <v>929</v>
       </c>
@@ -5479,7 +5602,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="16">
+    <row r="144" spans="1:4" ht="16">
       <c r="A144" s="83" t="s">
         <v>929</v>
       </c>
@@ -5497,6 +5620,9 @@
       <c r="C145" t="s">
         <v>951</v>
       </c>
+      <c r="D145" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="146" spans="1:5" ht="16">
       <c r="A146" s="83" t="s">
@@ -5505,6 +5631,12 @@
       <c r="B146" s="7" t="s">
         <v>731</v>
       </c>
+      <c r="C146" t="s">
+        <v>951</v>
+      </c>
+      <c r="D146" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="147" spans="1:5" ht="16">
       <c r="A147" s="83" t="s">
@@ -5532,6 +5664,12 @@
       <c r="B149" s="7" t="s">
         <v>734</v>
       </c>
+      <c r="C149" t="s">
+        <v>951</v>
+      </c>
+      <c r="D149" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="150" spans="1:5" ht="16">
       <c r="A150" s="83" t="s">
@@ -5548,11 +5686,14 @@
       <c r="B151" s="7" t="s">
         <v>736</v>
       </c>
+      <c r="C151" t="s">
+        <v>951</v>
+      </c>
       <c r="D151" t="s">
+        <v>953</v>
+      </c>
+      <c r="E151" t="s">
         <v>954</v>
-      </c>
-      <c r="E151" t="s">
-        <v>955</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="16">
@@ -5562,6 +5703,12 @@
       <c r="B152" s="7" t="s">
         <v>737</v>
       </c>
+      <c r="C152" t="s">
+        <v>951</v>
+      </c>
+      <c r="D152" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="153" spans="1:5" ht="16">
       <c r="A153" s="83" t="s">
@@ -5578,6 +5725,15 @@
       <c r="B154" s="7" t="s">
         <v>739</v>
       </c>
+      <c r="C154" t="s">
+        <v>951</v>
+      </c>
+      <c r="D154" t="s">
+        <v>961</v>
+      </c>
+      <c r="E154" t="s">
+        <v>968</v>
+      </c>
     </row>
     <row r="155" spans="1:5" ht="16">
       <c r="A155" s="83" t="s">
@@ -5586,6 +5742,12 @@
       <c r="B155" s="7" t="s">
         <v>740</v>
       </c>
+      <c r="C155" t="s">
+        <v>951</v>
+      </c>
+      <c r="D155" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="156" spans="1:5" ht="16">
       <c r="A156" s="83" t="s">
@@ -5626,6 +5788,12 @@
       <c r="B160" s="7" t="s">
         <v>745</v>
       </c>
+      <c r="C160" t="s">
+        <v>951</v>
+      </c>
+      <c r="D160" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="161" spans="1:4" ht="16">
       <c r="A161" s="83" t="s">
@@ -5650,6 +5818,12 @@
       <c r="B163" s="7" t="s">
         <v>748</v>
       </c>
+      <c r="C163" t="s">
+        <v>951</v>
+      </c>
+      <c r="D163" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="164" spans="1:4" ht="16">
       <c r="A164" s="83" t="s">
@@ -5658,6 +5832,12 @@
       <c r="B164" s="7" t="s">
         <v>749</v>
       </c>
+      <c r="C164" t="s">
+        <v>951</v>
+      </c>
+      <c r="D164" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="165" spans="1:4" ht="16">
       <c r="A165" s="83" t="s">
@@ -5666,6 +5846,12 @@
       <c r="B165" s="7" t="s">
         <v>932</v>
       </c>
+      <c r="C165" t="s">
+        <v>951</v>
+      </c>
+      <c r="D165" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="166" spans="1:4" ht="16">
       <c r="A166" s="83" t="s">
@@ -5674,6 +5860,12 @@
       <c r="B166" s="7" t="s">
         <v>750</v>
       </c>
+      <c r="C166" t="s">
+        <v>951</v>
+      </c>
+      <c r="D166" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="167" spans="1:4" ht="16">
       <c r="A167" s="83" t="s">
@@ -5682,6 +5874,12 @@
       <c r="B167" s="7" t="s">
         <v>751</v>
       </c>
+      <c r="C167" t="s">
+        <v>951</v>
+      </c>
+      <c r="D167" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="168" spans="1:4" ht="19">
       <c r="A168" s="83" t="s">
@@ -5706,8 +5904,11 @@
       <c r="B170" s="7" t="s">
         <v>753</v>
       </c>
+      <c r="C170" t="s">
+        <v>951</v>
+      </c>
       <c r="D170" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="16">
@@ -5733,6 +5934,12 @@
       <c r="B173" s="7" t="s">
         <v>756</v>
       </c>
+      <c r="C173" t="s">
+        <v>951</v>
+      </c>
+      <c r="D173" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="174" spans="1:4" ht="16">
       <c r="A174" s="83" t="s">
@@ -5757,6 +5964,12 @@
       <c r="B176" s="7" t="s">
         <v>759</v>
       </c>
+      <c r="C176" t="s">
+        <v>951</v>
+      </c>
+      <c r="D176" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="177" spans="1:5" ht="16">
       <c r="A177" s="83" t="s">
@@ -5797,6 +6010,12 @@
       <c r="B181" s="7" t="s">
         <v>764</v>
       </c>
+      <c r="C181" t="s">
+        <v>951</v>
+      </c>
+      <c r="D181" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="182" spans="1:5" ht="16">
       <c r="A182" s="83" t="s">
@@ -5813,6 +6032,12 @@
       <c r="B183" s="7" t="s">
         <v>766</v>
       </c>
+      <c r="C183" t="s">
+        <v>951</v>
+      </c>
+      <c r="D183" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="184" spans="1:5" ht="16">
       <c r="A184" s="83" t="s">
@@ -5821,6 +6046,12 @@
       <c r="B184" s="7" t="s">
         <v>767</v>
       </c>
+      <c r="C184" t="s">
+        <v>951</v>
+      </c>
+      <c r="D184" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="185" spans="1:5" ht="16">
       <c r="A185" s="83" t="s">
@@ -5853,11 +6084,14 @@
       <c r="B188" s="7" t="s">
         <v>771</v>
       </c>
+      <c r="C188" t="s">
+        <v>951</v>
+      </c>
       <c r="D188" t="s">
-        <v>958</v>
+        <v>969</v>
       </c>
       <c r="E188" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="189" spans="1:5" ht="16">
@@ -5867,11 +6101,14 @@
       <c r="B189" s="7" t="s">
         <v>772</v>
       </c>
+      <c r="C189" t="s">
+        <v>951</v>
+      </c>
       <c r="D189" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="E189" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="190" spans="1:5" ht="16">
@@ -5897,8 +6134,14 @@
       <c r="B192" s="7" t="s">
         <v>775</v>
       </c>
-    </row>
-    <row r="193" spans="1:2" ht="16">
+      <c r="C192" t="s">
+        <v>951</v>
+      </c>
+      <c r="D192" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" ht="16">
       <c r="A193" s="83" t="s">
         <v>929</v>
       </c>
@@ -5906,15 +6149,21 @@
         <v>776</v>
       </c>
     </row>
-    <row r="194" spans="1:2" ht="16">
+    <row r="194" spans="1:4" ht="16">
       <c r="A194" s="83" t="s">
         <v>929</v>
       </c>
       <c r="B194" s="7" t="s">
         <v>777</v>
       </c>
-    </row>
-    <row r="195" spans="1:2" ht="16">
+      <c r="C194" t="s">
+        <v>951</v>
+      </c>
+      <c r="D194" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" ht="16">
       <c r="A195" s="83" t="s">
         <v>929</v>
       </c>
@@ -5922,7 +6171,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="16">
+    <row r="196" spans="1:4" ht="16">
       <c r="A196" s="83" t="s">
         <v>929</v>
       </c>
@@ -5930,15 +6179,21 @@
         <v>778</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="16">
+    <row r="197" spans="1:4" ht="16">
       <c r="A197" s="83" t="s">
         <v>929</v>
       </c>
       <c r="B197" s="7" t="s">
         <v>779</v>
       </c>
-    </row>
-    <row r="198" spans="1:2" ht="16">
+      <c r="C197" t="s">
+        <v>951</v>
+      </c>
+      <c r="D197" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" ht="16">
       <c r="A198" s="83" t="s">
         <v>929</v>
       </c>
@@ -5946,7 +6201,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="199" spans="1:2" ht="19">
+    <row r="199" spans="1:4" ht="19">
       <c r="A199" s="83" t="s">
         <v>929</v>
       </c>
@@ -5954,7 +6209,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="200" spans="1:2" ht="16">
+    <row r="200" spans="1:4" ht="16">
       <c r="A200" s="83" t="s">
         <v>929</v>
       </c>
@@ -5962,15 +6217,21 @@
         <v>782</v>
       </c>
     </row>
-    <row r="201" spans="1:2" ht="16">
+    <row r="201" spans="1:4" ht="16">
       <c r="A201" s="83" t="s">
         <v>929</v>
       </c>
       <c r="B201" s="88" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="202" spans="1:2" ht="16">
+      <c r="C201" t="s">
+        <v>951</v>
+      </c>
+      <c r="D201" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" ht="16">
       <c r="A202" s="83" t="s">
         <v>929</v>
       </c>
@@ -5978,7 +6239,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="203" spans="1:2" ht="16">
+    <row r="203" spans="1:4" ht="16">
       <c r="A203" s="83" t="s">
         <v>929</v>
       </c>
@@ -5986,7 +6247,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="204" spans="1:2" ht="16">
+    <row r="204" spans="1:4" ht="16">
       <c r="A204" s="83" t="s">
         <v>929</v>
       </c>
@@ -5994,7 +6255,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="205" spans="1:2" ht="16">
+    <row r="205" spans="1:4" ht="16">
       <c r="A205" s="83" t="s">
         <v>929</v>
       </c>
@@ -6002,7 +6263,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="206" spans="1:2" ht="16">
+    <row r="206" spans="1:4" ht="16">
       <c r="A206" s="83" t="s">
         <v>929</v>
       </c>
@@ -6010,7 +6271,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="207" spans="1:2" ht="16">
+    <row r="207" spans="1:4" ht="16">
       <c r="A207" s="83" t="s">
         <v>929</v>
       </c>
@@ -6018,7 +6279,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="208" spans="1:2" ht="16">
+    <row r="208" spans="1:4" ht="16">
       <c r="A208" s="83" t="s">
         <v>929</v>
       </c>
@@ -6076,6 +6337,12 @@
       <c r="B214" s="7" t="s">
         <v>796</v>
       </c>
+      <c r="C214" t="s">
+        <v>951</v>
+      </c>
+      <c r="D214" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="215" spans="1:5" ht="16">
       <c r="A215" s="83" t="s">
@@ -6084,11 +6351,14 @@
       <c r="B215" s="7" t="s">
         <v>797</v>
       </c>
+      <c r="C215" t="s">
+        <v>951</v>
+      </c>
       <c r="D215" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="E215" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="216" spans="1:5" ht="16">
@@ -6098,6 +6368,12 @@
       <c r="B216" s="7" t="s">
         <v>798</v>
       </c>
+      <c r="C216" t="s">
+        <v>951</v>
+      </c>
+      <c r="D216" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="217" spans="1:5" ht="16">
       <c r="A217" s="83" t="s">
@@ -6122,11 +6398,14 @@
       <c r="B219" s="7" t="s">
         <v>801</v>
       </c>
+      <c r="C219" t="s">
+        <v>951</v>
+      </c>
       <c r="D219" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="E219" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="220" spans="1:5" ht="16">
@@ -6169,7 +6448,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="225" spans="1:2" ht="16">
+    <row r="225" spans="1:4" ht="16">
       <c r="A225" s="83" t="s">
         <v>589</v>
       </c>
@@ -6177,23 +6456,35 @@
         <v>807</v>
       </c>
     </row>
-    <row r="226" spans="1:2" ht="16">
+    <row r="226" spans="1:4" ht="16">
       <c r="A226" s="83" t="s">
         <v>589</v>
       </c>
       <c r="B226" s="7" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="227" spans="1:2" ht="16">
+      <c r="C226" t="s">
+        <v>951</v>
+      </c>
+      <c r="D226" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" ht="16">
       <c r="A227" s="83" t="s">
         <v>589</v>
       </c>
       <c r="B227" s="7" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="228" spans="1:2" ht="19">
+      <c r="C227" t="s">
+        <v>951</v>
+      </c>
+      <c r="D227" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" ht="19">
       <c r="A228" s="83" t="s">
         <v>589</v>
       </c>
@@ -6201,7 +6492,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="229" spans="1:2" ht="16">
+    <row r="229" spans="1:4" ht="16">
       <c r="A229" s="83" t="s">
         <v>589</v>
       </c>
@@ -6209,7 +6500,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="230" spans="1:2" ht="16">
+    <row r="230" spans="1:4" ht="16">
       <c r="A230" s="83" t="s">
         <v>589</v>
       </c>
@@ -6217,23 +6508,35 @@
         <v>811</v>
       </c>
     </row>
-    <row r="231" spans="1:2" ht="16">
+    <row r="231" spans="1:4" ht="16">
       <c r="A231" s="83" t="s">
         <v>589</v>
       </c>
       <c r="B231" s="7" t="s">
         <v>812</v>
       </c>
-    </row>
-    <row r="232" spans="1:2" ht="16">
+      <c r="C231" t="s">
+        <v>951</v>
+      </c>
+      <c r="D231" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" ht="16">
       <c r="A232" s="83" t="s">
         <v>589</v>
       </c>
       <c r="B232" s="7" t="s">
         <v>813</v>
       </c>
-    </row>
-    <row r="233" spans="1:2" ht="19">
+      <c r="C232" t="s">
+        <v>951</v>
+      </c>
+      <c r="D232" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" ht="19">
       <c r="A233" s="83" t="s">
         <v>589</v>
       </c>
@@ -6241,7 +6544,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="234" spans="1:2" ht="16">
+    <row r="234" spans="1:4" ht="16">
       <c r="A234" s="83" t="s">
         <v>589</v>
       </c>
@@ -6249,7 +6552,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="235" spans="1:2" ht="16">
+    <row r="235" spans="1:4" ht="16">
       <c r="A235" s="83" t="s">
         <v>589</v>
       </c>
@@ -6257,7 +6560,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="236" spans="1:2" ht="16">
+    <row r="236" spans="1:4" ht="16">
       <c r="A236" s="83" t="s">
         <v>589</v>
       </c>
@@ -6265,7 +6568,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="237" spans="1:2" ht="16">
+    <row r="237" spans="1:4" ht="16">
       <c r="A237" s="83" t="s">
         <v>589</v>
       </c>
@@ -6273,7 +6576,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="238" spans="1:2" ht="16">
+    <row r="238" spans="1:4" ht="16">
       <c r="A238" s="83" t="s">
         <v>589</v>
       </c>
@@ -6281,7 +6584,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="239" spans="1:2" ht="16">
+    <row r="239" spans="1:4" ht="16">
       <c r="A239" s="83" t="s">
         <v>589</v>
       </c>
@@ -6289,7 +6592,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="240" spans="1:2" ht="16">
+    <row r="240" spans="1:4" ht="16">
       <c r="A240" s="83" t="s">
         <v>589</v>
       </c>
@@ -6387,6 +6690,12 @@
       <c r="B251" s="7" t="s">
         <v>831</v>
       </c>
+      <c r="C251" t="s">
+        <v>951</v>
+      </c>
+      <c r="D251" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="252" spans="1:5" ht="16">
       <c r="A252" s="83" t="s">
@@ -6428,15 +6737,21 @@
         <v>835</v>
       </c>
     </row>
-    <row r="257" spans="1:2" ht="16">
+    <row r="257" spans="1:4" ht="16">
       <c r="A257" s="83" t="s">
         <v>590</v>
       </c>
       <c r="B257" s="7" t="s">
         <v>836</v>
       </c>
-    </row>
-    <row r="258" spans="1:2" ht="16">
+      <c r="C257" t="s">
+        <v>951</v>
+      </c>
+      <c r="D257" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" ht="16">
       <c r="A258" s="83" t="s">
         <v>590</v>
       </c>
@@ -6444,7 +6759,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="259" spans="1:2" ht="16">
+    <row r="259" spans="1:4" ht="16">
       <c r="A259" s="83" t="s">
         <v>590</v>
       </c>
@@ -6452,7 +6767,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="260" spans="1:2" ht="16">
+    <row r="260" spans="1:4" ht="16">
       <c r="A260" s="83" t="s">
         <v>590</v>
       </c>
@@ -6460,7 +6775,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="261" spans="1:2" ht="16">
+    <row r="261" spans="1:4" ht="16">
       <c r="A261" s="83" t="s">
         <v>590</v>
       </c>
@@ -6468,15 +6783,21 @@
         <v>840</v>
       </c>
     </row>
-    <row r="262" spans="1:2" ht="16">
+    <row r="262" spans="1:4" ht="16">
       <c r="A262" s="83" t="s">
         <v>590</v>
       </c>
       <c r="B262" s="7" t="s">
         <v>841</v>
       </c>
-    </row>
-    <row r="263" spans="1:2" ht="16">
+      <c r="C262" t="s">
+        <v>951</v>
+      </c>
+      <c r="D262" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" ht="16">
       <c r="A263" s="83" t="s">
         <v>590</v>
       </c>
@@ -6484,7 +6805,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="264" spans="1:2" ht="16">
+    <row r="264" spans="1:4" ht="16">
       <c r="A264" s="83" t="s">
         <v>590</v>
       </c>
@@ -6492,23 +6813,35 @@
         <v>843</v>
       </c>
     </row>
-    <row r="265" spans="1:2" ht="16">
+    <row r="265" spans="1:4" ht="16">
       <c r="A265" s="83" t="s">
         <v>590</v>
       </c>
       <c r="B265" s="7" t="s">
         <v>844</v>
       </c>
-    </row>
-    <row r="266" spans="1:2" ht="16">
+      <c r="C265" t="s">
+        <v>951</v>
+      </c>
+      <c r="D265" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" ht="16">
       <c r="A266" s="83" t="s">
         <v>590</v>
       </c>
       <c r="B266" s="7" t="s">
         <v>845</v>
       </c>
-    </row>
-    <row r="267" spans="1:2" ht="16">
+      <c r="C266" t="s">
+        <v>951</v>
+      </c>
+      <c r="D266" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" ht="16">
       <c r="A267" s="83" t="s">
         <v>590</v>
       </c>
@@ -6516,44 +6849,74 @@
         <v>846</v>
       </c>
     </row>
-    <row r="268" spans="1:2" ht="16">
+    <row r="268" spans="1:4" ht="16">
       <c r="A268" s="83" t="s">
         <v>590</v>
       </c>
       <c r="B268" s="7" t="s">
         <v>847</v>
       </c>
-    </row>
-    <row r="269" spans="1:2" ht="16">
+      <c r="C268" t="s">
+        <v>951</v>
+      </c>
+      <c r="D268" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" ht="16">
       <c r="A269" s="83" t="s">
         <v>590</v>
       </c>
       <c r="B269" s="7" t="s">
         <v>848</v>
       </c>
-    </row>
-    <row r="270" spans="1:2" ht="16">
+      <c r="C269" t="s">
+        <v>951</v>
+      </c>
+      <c r="D269" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" ht="16">
       <c r="A270" s="83" t="s">
         <v>590</v>
       </c>
       <c r="B270" s="7" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="271" spans="1:2" ht="16">
+      <c r="C270" t="s">
+        <v>951</v>
+      </c>
+      <c r="D270" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" ht="16">
       <c r="A271" s="83" t="s">
         <v>590</v>
       </c>
       <c r="B271" s="7" t="s">
         <v>850</v>
       </c>
-    </row>
-    <row r="272" spans="1:2" ht="16">
+      <c r="C271" t="s">
+        <v>951</v>
+      </c>
+      <c r="D271" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" ht="16">
       <c r="A272" s="83" t="s">
         <v>590</v>
       </c>
       <c r="B272" s="7" t="s">
         <v>851</v>
+      </c>
+      <c r="C272" t="s">
+        <v>951</v>
+      </c>
+      <c r="D272" t="s">
+        <v>961</v>
       </c>
     </row>
     <row r="273" spans="1:5" ht="16">
@@ -6563,6 +6926,12 @@
       <c r="B273" s="7" t="s">
         <v>852</v>
       </c>
+      <c r="C273" t="s">
+        <v>951</v>
+      </c>
+      <c r="D273" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="274" spans="1:5" ht="16">
       <c r="A274" s="83" t="s">
@@ -6570,6 +6939,12 @@
       </c>
       <c r="B274" s="7" t="s">
         <v>853</v>
+      </c>
+      <c r="C274" t="s">
+        <v>951</v>
+      </c>
+      <c r="D274" t="s">
+        <v>961</v>
       </c>
     </row>
     <row r="275" spans="1:5" ht="19">
@@ -6687,7 +7062,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="289" spans="1:3" ht="16">
+    <row r="289" spans="1:4" ht="16">
       <c r="A289" s="83" t="s">
         <v>930</v>
       </c>
@@ -6695,7 +7070,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="290" spans="1:3" ht="16">
+    <row r="290" spans="1:4" ht="16">
       <c r="A290" s="83" t="s">
         <v>930</v>
       </c>
@@ -6703,7 +7078,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="291" spans="1:3" ht="16">
+    <row r="291" spans="1:4" ht="16">
       <c r="A291" s="83" t="s">
         <v>930</v>
       </c>
@@ -6711,7 +7086,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="292" spans="1:3" ht="16">
+    <row r="292" spans="1:4" ht="16">
       <c r="A292" s="83" t="s">
         <v>930</v>
       </c>
@@ -6719,7 +7094,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="293" spans="1:3" ht="16">
+    <row r="293" spans="1:4" ht="16">
       <c r="A293" s="83" t="s">
         <v>930</v>
       </c>
@@ -6727,7 +7102,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="294" spans="1:3" ht="16">
+    <row r="294" spans="1:4" ht="16">
       <c r="A294" s="83" t="s">
         <v>930</v>
       </c>
@@ -6735,7 +7110,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="295" spans="1:3" ht="16">
+    <row r="295" spans="1:4" ht="16">
       <c r="A295" s="83" t="s">
         <v>930</v>
       </c>
@@ -6743,15 +7118,21 @@
         <v>874</v>
       </c>
     </row>
-    <row r="296" spans="1:3" ht="16">
+    <row r="296" spans="1:4" ht="16">
       <c r="A296" s="83" t="s">
         <v>930</v>
       </c>
       <c r="B296" s="7" t="s">
         <v>875</v>
       </c>
-    </row>
-    <row r="297" spans="1:3" ht="16">
+      <c r="C296" t="s">
+        <v>951</v>
+      </c>
+      <c r="D296" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" ht="16">
       <c r="A297" s="83" t="s">
         <v>930</v>
       </c>
@@ -6759,7 +7140,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="298" spans="1:3" ht="19">
+    <row r="298" spans="1:4" ht="19">
       <c r="A298" s="83" t="s">
         <v>930</v>
       </c>
@@ -6767,7 +7148,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="299" spans="1:3" ht="16">
+    <row r="299" spans="1:4" ht="16">
       <c r="A299" s="83" t="s">
         <v>930</v>
       </c>
@@ -6775,7 +7156,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="300" spans="1:3" ht="16">
+    <row r="300" spans="1:4" ht="16">
       <c r="A300" s="83" t="s">
         <v>930</v>
       </c>
@@ -6785,81 +7166,105 @@
       <c r="C300" t="s">
         <v>951</v>
       </c>
-    </row>
-    <row r="301" spans="1:3" ht="16">
+      <c r="D300" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" ht="16">
       <c r="A301" s="83" t="s">
         <v>930</v>
       </c>
       <c r="B301" s="7" t="s">
         <v>879</v>
       </c>
-      <c r="C301" t="s">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="302" spans="1:3" ht="16">
+    </row>
+    <row r="302" spans="1:4" ht="16">
       <c r="A302" s="83" t="s">
         <v>930</v>
       </c>
       <c r="B302" s="7" t="s">
         <v>880</v>
       </c>
-      <c r="C302" t="s">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="303" spans="1:3" ht="16">
+    </row>
+    <row r="303" spans="1:4" ht="16">
       <c r="A303" s="83" t="s">
         <v>930</v>
       </c>
       <c r="B303" s="7" t="s">
         <v>881</v>
       </c>
-      <c r="C303" t="s">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="304" spans="1:3" ht="16">
+    </row>
+    <row r="304" spans="1:4" ht="16">
       <c r="A304" s="83" t="s">
         <v>930</v>
       </c>
       <c r="B304" s="7" t="s">
         <v>882</v>
       </c>
-    </row>
-    <row r="305" spans="1:2" ht="16">
+      <c r="C304" t="s">
+        <v>951</v>
+      </c>
+      <c r="D304" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" ht="16">
       <c r="A305" s="83" t="s">
         <v>930</v>
       </c>
       <c r="B305" s="7" t="s">
         <v>883</v>
       </c>
-    </row>
-    <row r="306" spans="1:2" ht="16">
+      <c r="C305" t="s">
+        <v>951</v>
+      </c>
+      <c r="D305" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5" ht="16">
       <c r="A306" s="83" t="s">
         <v>930</v>
       </c>
       <c r="B306" s="7" t="s">
         <v>884</v>
       </c>
-    </row>
-    <row r="307" spans="1:2" ht="16">
+      <c r="C306" t="s">
+        <v>951</v>
+      </c>
+      <c r="D306" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5" ht="16">
       <c r="A307" s="83" t="s">
         <v>930</v>
       </c>
       <c r="B307" s="7" t="s">
         <v>885</v>
       </c>
-    </row>
-    <row r="308" spans="1:2" ht="16">
+      <c r="C307" t="s">
+        <v>951</v>
+      </c>
+      <c r="D307" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5" ht="16">
       <c r="A308" s="83" t="s">
         <v>930</v>
       </c>
       <c r="B308" s="7" t="s">
         <v>886</v>
       </c>
-    </row>
-    <row r="309" spans="1:2" ht="19">
+      <c r="C308" t="s">
+        <v>951</v>
+      </c>
+      <c r="D308" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="309" spans="1:5" ht="19">
       <c r="A309" s="83" t="s">
         <v>930</v>
       </c>
@@ -6867,7 +7272,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="310" spans="1:2" ht="16">
+    <row r="310" spans="1:5" ht="16">
       <c r="A310" s="83" t="s">
         <v>930</v>
       </c>
@@ -6875,23 +7280,38 @@
         <v>888</v>
       </c>
     </row>
-    <row r="311" spans="1:2" ht="16">
+    <row r="311" spans="1:5" ht="16">
       <c r="A311" s="83" t="s">
         <v>930</v>
       </c>
       <c r="B311" s="7" t="s">
         <v>889</v>
       </c>
-    </row>
-    <row r="312" spans="1:2" ht="16">
+      <c r="C311" t="s">
+        <v>951</v>
+      </c>
+      <c r="D311" t="s">
+        <v>961</v>
+      </c>
+      <c r="E311" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="312" spans="1:5" ht="16">
       <c r="A312" s="83" t="s">
         <v>930</v>
       </c>
       <c r="B312" s="7" t="s">
         <v>890</v>
       </c>
-    </row>
-    <row r="313" spans="1:2" ht="16">
+      <c r="C312" t="s">
+        <v>951</v>
+      </c>
+      <c r="D312" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="313" spans="1:5" ht="16">
       <c r="A313" s="83" t="s">
         <v>930</v>
       </c>
@@ -6899,7 +7319,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="314" spans="1:2" ht="16">
+    <row r="314" spans="1:5" ht="16">
       <c r="A314" s="83" t="s">
         <v>930</v>
       </c>
@@ -6907,7 +7327,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="315" spans="1:2" ht="16">
+    <row r="315" spans="1:5" ht="16">
       <c r="A315" s="83" t="s">
         <v>930</v>
       </c>
@@ -6915,7 +7335,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="316" spans="1:2" ht="16">
+    <row r="316" spans="1:5" ht="16">
       <c r="A316" s="83" t="s">
         <v>930</v>
       </c>
@@ -6923,7 +7343,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="317" spans="1:2" ht="16">
+    <row r="317" spans="1:5" ht="16">
       <c r="A317" s="83" t="s">
         <v>930</v>
       </c>
@@ -6931,7 +7351,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="318" spans="1:2" ht="16">
+    <row r="318" spans="1:5" ht="16">
       <c r="A318" s="83" t="s">
         <v>930</v>
       </c>
@@ -6939,7 +7359,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="319" spans="1:2" ht="16">
+    <row r="319" spans="1:5" ht="16">
       <c r="A319" s="83" t="s">
         <v>930</v>
       </c>
@@ -6947,7 +7367,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="320" spans="1:2" ht="16">
+    <row r="320" spans="1:5" ht="16">
       <c r="A320" s="83" t="s">
         <v>930</v>
       </c>
@@ -6955,7 +7375,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="321" spans="1:2" ht="16">
+    <row r="321" spans="1:5" ht="16">
       <c r="A321" s="83" t="s">
         <v>930</v>
       </c>
@@ -6963,7 +7383,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="322" spans="1:2" ht="16">
+    <row r="322" spans="1:5" ht="16">
       <c r="A322" s="83" t="s">
         <v>930</v>
       </c>
@@ -6971,7 +7391,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="323" spans="1:2" ht="16">
+    <row r="323" spans="1:5" ht="16">
       <c r="A323" s="83" t="s">
         <v>930</v>
       </c>
@@ -6979,23 +7399,35 @@
         <v>901</v>
       </c>
     </row>
-    <row r="324" spans="1:2" ht="16">
+    <row r="324" spans="1:5" ht="16">
       <c r="A324" s="83" t="s">
         <v>930</v>
       </c>
       <c r="B324" s="7" t="s">
         <v>902</v>
       </c>
-    </row>
-    <row r="325" spans="1:2" ht="16">
+      <c r="C324" t="s">
+        <v>951</v>
+      </c>
+      <c r="D324" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="325" spans="1:5" ht="16">
       <c r="A325" s="83" t="s">
         <v>930</v>
       </c>
       <c r="B325" s="7" t="s">
         <v>903</v>
       </c>
-    </row>
-    <row r="326" spans="1:2" ht="19">
+      <c r="C325" t="s">
+        <v>951</v>
+      </c>
+      <c r="D325" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="326" spans="1:5" ht="19">
       <c r="A326" s="83" t="s">
         <v>930</v>
       </c>
@@ -7003,7 +7435,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="327" spans="1:2" ht="16">
+    <row r="327" spans="1:5" ht="16">
       <c r="A327" s="83" t="s">
         <v>930</v>
       </c>
@@ -7011,15 +7443,24 @@
         <v>905</v>
       </c>
     </row>
-    <row r="328" spans="1:2" ht="16">
+    <row r="328" spans="1:5" ht="16">
       <c r="A328" s="83" t="s">
         <v>930</v>
       </c>
       <c r="B328" s="7" t="s">
         <v>906</v>
       </c>
-    </row>
-    <row r="329" spans="1:2" ht="16">
+      <c r="C328" t="s">
+        <v>951</v>
+      </c>
+      <c r="D328" t="s">
+        <v>961</v>
+      </c>
+      <c r="E328" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="329" spans="1:5" ht="16">
       <c r="A329" s="83" t="s">
         <v>930</v>
       </c>
@@ -7027,7 +7468,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="330" spans="1:2" ht="16">
+    <row r="330" spans="1:5" ht="16">
       <c r="A330" s="83" t="s">
         <v>930</v>
       </c>
@@ -7035,15 +7476,21 @@
         <v>908</v>
       </c>
     </row>
-    <row r="331" spans="1:2" ht="16">
+    <row r="331" spans="1:5" ht="16">
       <c r="A331" s="83" t="s">
         <v>930</v>
       </c>
       <c r="B331" s="7" t="s">
         <v>909</v>
       </c>
-    </row>
-    <row r="332" spans="1:2" ht="16">
+      <c r="C331" t="s">
+        <v>951</v>
+      </c>
+      <c r="D331" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="332" spans="1:5" ht="16">
       <c r="A332" s="83" t="s">
         <v>930</v>
       </c>
@@ -7051,31 +7498,49 @@
         <v>910</v>
       </c>
     </row>
-    <row r="333" spans="1:2" ht="16">
+    <row r="333" spans="1:5" ht="16">
       <c r="A333" s="83" t="s">
         <v>930</v>
       </c>
       <c r="B333" s="7" t="s">
         <v>911</v>
       </c>
-    </row>
-    <row r="334" spans="1:2" ht="16">
+      <c r="C333" t="s">
+        <v>951</v>
+      </c>
+      <c r="D333" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="334" spans="1:5" ht="16">
       <c r="A334" s="83" t="s">
         <v>930</v>
       </c>
       <c r="B334" s="7" t="s">
         <v>912</v>
       </c>
-    </row>
-    <row r="335" spans="1:2" ht="16">
+      <c r="C334" t="s">
+        <v>951</v>
+      </c>
+      <c r="D334" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="335" spans="1:5" ht="16">
       <c r="A335" s="83" t="s">
         <v>930</v>
       </c>
       <c r="B335" s="7" t="s">
         <v>913</v>
       </c>
-    </row>
-    <row r="336" spans="1:2" ht="16">
+      <c r="C335" t="s">
+        <v>951</v>
+      </c>
+      <c r="D335" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="336" spans="1:5" ht="16">
       <c r="A336" s="83" t="s">
         <v>930</v>
       </c>
@@ -7083,15 +7548,21 @@
         <v>914</v>
       </c>
     </row>
-    <row r="337" spans="1:2" ht="16">
+    <row r="337" spans="1:4" ht="16">
       <c r="A337" s="83" t="s">
         <v>930</v>
       </c>
       <c r="B337" s="7" t="s">
         <v>915</v>
       </c>
-    </row>
-    <row r="338" spans="1:2" ht="19">
+      <c r="C337" t="s">
+        <v>951</v>
+      </c>
+      <c r="D337" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" ht="19">
       <c r="A338" s="83" t="s">
         <v>930</v>
       </c>
@@ -7099,7 +7570,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="339" spans="1:2" ht="16">
+    <row r="339" spans="1:4" ht="16">
       <c r="A339" s="83" t="s">
         <v>930</v>
       </c>
@@ -7107,7 +7578,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="340" spans="1:2" ht="16">
+    <row r="340" spans="1:4" ht="16">
       <c r="A340" s="83" t="s">
         <v>930</v>
       </c>
@@ -7115,7 +7586,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="341" spans="1:2" ht="16">
+    <row r="341" spans="1:4" ht="16">
       <c r="A341" s="83" t="s">
         <v>930</v>
       </c>
@@ -7123,7 +7594,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="342" spans="1:2" ht="16">
+    <row r="342" spans="1:4" ht="16">
       <c r="A342" s="83" t="s">
         <v>930</v>
       </c>
@@ -7131,7 +7602,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="343" spans="1:2" ht="16">
+    <row r="343" spans="1:4" ht="16">
       <c r="A343" s="83" t="s">
         <v>930</v>
       </c>
@@ -7139,7 +7610,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="344" spans="1:2" ht="16">
+    <row r="344" spans="1:4" ht="16">
       <c r="A344" s="83" t="s">
         <v>930</v>
       </c>
@@ -7147,7 +7618,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="345" spans="1:2" ht="16">
+    <row r="345" spans="1:4" ht="16">
       <c r="A345" s="83" t="s">
         <v>930</v>
       </c>
@@ -7155,7 +7626,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="346" spans="1:2" ht="16">
+    <row r="346" spans="1:4" ht="16">
       <c r="A346" s="83" t="s">
         <v>930</v>
       </c>
@@ -7163,7 +7634,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="347" spans="1:2" ht="16">
+    <row r="347" spans="1:4" ht="16">
       <c r="A347" s="83" t="s">
         <v>930</v>
       </c>
@@ -7171,7 +7642,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="348" spans="1:2" ht="16">
+    <row r="348" spans="1:4" ht="16">
       <c r="A348" s="83" t="s">
         <v>930</v>
       </c>
@@ -7179,7 +7650,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="349" spans="1:2" ht="16">
+    <row r="349" spans="1:4" ht="16">
       <c r="A349" s="83" t="s">
         <v>930</v>
       </c>
@@ -7281,7 +7752,7 @@
       </c>
       <c r="F1" s="90">
         <f ca="1">(TODAY()-H1)*-1</f>
-        <v>-187</v>
+        <v>-190</v>
       </c>
       <c r="G1" s="91" t="s">
         <v>10</v>
@@ -15001,12 +15472,12 @@
       <c r="M1" s="16"/>
     </row>
     <row r="2" spans="1:13" s="18" customFormat="1" ht="26" customHeight="1">
-      <c r="A2" s="125"/>
-      <c r="B2" s="125"/>
-      <c r="C2" s="125"/>
-      <c r="D2" s="125"/>
-      <c r="E2" s="125"/>
-      <c r="F2" s="125"/>
+      <c r="A2" s="98"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
       <c r="G2" s="49" t="s">
         <v>501</v>
       </c>
@@ -15030,14 +15501,14 @@
       </c>
     </row>
     <row r="3" spans="1:13" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A3" s="126" t="s">
+      <c r="A3" s="99" t="s">
         <v>446</v>
       </c>
-      <c r="B3" s="127"/>
-      <c r="C3" s="127"/>
-      <c r="D3" s="127"/>
-      <c r="E3" s="127"/>
-      <c r="F3" s="127"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
       <c r="G3" s="27"/>
       <c r="H3" s="23"/>
       <c r="I3" s="24" t="s">
@@ -15048,12 +15519,12 @@
       <c r="M3" s="26"/>
     </row>
     <row r="4" spans="1:13" s="32" customFormat="1" ht="14" customHeight="1">
-      <c r="A4" s="127"/>
-      <c r="B4" s="127"/>
-      <c r="C4" s="127"/>
-      <c r="D4" s="127"/>
-      <c r="E4" s="127"/>
-      <c r="F4" s="127"/>
+      <c r="A4" s="100"/>
+      <c r="B4" s="100"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="100"/>
       <c r="G4" s="27"/>
       <c r="H4" s="27"/>
       <c r="I4" s="27"/>
@@ -15080,16 +15551,16 @@
       <c r="M5" s="40"/>
     </row>
     <row r="6" spans="1:13" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="101" t="s">
         <v>448</v>
       </c>
-      <c r="B6" s="100" t="s">
+      <c r="B6" s="101" t="s">
         <v>449</v>
       </c>
-      <c r="C6" s="100" t="s">
+      <c r="C6" s="101" t="s">
         <v>450</v>
       </c>
-      <c r="D6" s="115" t="s">
+      <c r="D6" s="105" t="s">
         <v>505</v>
       </c>
       <c r="E6" s="41" t="s">
@@ -15111,18 +15582,18 @@
       <c r="K6" s="43" t="s">
         <v>454</v>
       </c>
-      <c r="L6" s="112" t="s">
+      <c r="L6" s="109" t="s">
         <v>507</v>
       </c>
-      <c r="M6" s="112" t="s">
+      <c r="M6" s="109" t="s">
         <v>455</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A7" s="101"/>
-      <c r="B7" s="101"/>
-      <c r="C7" s="101"/>
-      <c r="D7" s="116"/>
+      <c r="A7" s="102"/>
+      <c r="B7" s="102"/>
+      <c r="C7" s="102"/>
+      <c r="D7" s="106"/>
       <c r="E7" s="41" t="s">
         <v>456</v>
       </c>
@@ -15144,22 +15615,22 @@
       <c r="K7" s="43" t="s">
         <v>458</v>
       </c>
-      <c r="L7" s="113"/>
-      <c r="M7" s="113"/>
+      <c r="L7" s="110"/>
+      <c r="M7" s="110"/>
     </row>
     <row r="8" spans="1:13" s="18" customFormat="1" ht="18" customHeight="1" outlineLevel="1">
-      <c r="A8" s="101"/>
-      <c r="B8" s="101"/>
-      <c r="C8" s="101"/>
-      <c r="D8" s="116"/>
-      <c r="E8" s="100" t="s">
+      <c r="A8" s="102"/>
+      <c r="B8" s="102"/>
+      <c r="C8" s="102"/>
+      <c r="D8" s="106"/>
+      <c r="E8" s="101" t="s">
         <v>459</v>
       </c>
-      <c r="F8" s="103" t="s">
+      <c r="F8" s="112" t="s">
         <v>511</v>
       </c>
       <c r="G8" s="78"/>
-      <c r="H8" s="106" t="s">
+      <c r="H8" s="115" t="s">
         <v>512</v>
       </c>
       <c r="I8" s="50" t="s">
@@ -15171,18 +15642,18 @@
       <c r="K8" s="43" t="s">
         <v>466</v>
       </c>
-      <c r="L8" s="113"/>
-      <c r="M8" s="113"/>
+      <c r="L8" s="110"/>
+      <c r="M8" s="110"/>
     </row>
     <row r="9" spans="1:13" s="18" customFormat="1" ht="16" customHeight="1" outlineLevel="1">
-      <c r="A9" s="101"/>
-      <c r="B9" s="101"/>
-      <c r="C9" s="101"/>
-      <c r="D9" s="116"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="104"/>
+      <c r="A9" s="102"/>
+      <c r="B9" s="102"/>
+      <c r="C9" s="102"/>
+      <c r="D9" s="106"/>
+      <c r="E9" s="102"/>
+      <c r="F9" s="113"/>
       <c r="G9" s="79"/>
-      <c r="H9" s="107"/>
+      <c r="H9" s="116"/>
       <c r="I9" s="50" t="s">
         <v>514</v>
       </c>
@@ -15190,41 +15661,41 @@
       <c r="K9" s="51" t="s">
         <v>515</v>
       </c>
-      <c r="L9" s="113"/>
-      <c r="M9" s="113"/>
+      <c r="L9" s="110"/>
+      <c r="M9" s="110"/>
     </row>
     <row r="10" spans="1:13" s="18" customFormat="1" ht="19" customHeight="1" outlineLevel="1">
-      <c r="A10" s="101"/>
-      <c r="B10" s="101"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="116"/>
-      <c r="E10" s="102"/>
-      <c r="F10" s="105"/>
+      <c r="A10" s="102"/>
+      <c r="B10" s="102"/>
+      <c r="C10" s="102"/>
+      <c r="D10" s="106"/>
+      <c r="E10" s="103"/>
+      <c r="F10" s="114"/>
       <c r="G10" s="58" t="s">
         <v>582</v>
       </c>
-      <c r="H10" s="108"/>
+      <c r="H10" s="117"/>
       <c r="I10" s="50" t="s">
         <v>516</v>
       </c>
       <c r="J10" s="44"/>
       <c r="K10" s="52"/>
-      <c r="L10" s="113"/>
-      <c r="M10" s="113"/>
+      <c r="L10" s="110"/>
+      <c r="M10" s="110"/>
     </row>
     <row r="11" spans="1:13" s="18" customFormat="1" ht="13" customHeight="1" outlineLevel="1">
-      <c r="A11" s="101"/>
-      <c r="B11" s="101"/>
-      <c r="C11" s="101"/>
-      <c r="D11" s="116"/>
-      <c r="E11" s="100" t="s">
+      <c r="A11" s="102"/>
+      <c r="B11" s="102"/>
+      <c r="C11" s="102"/>
+      <c r="D11" s="106"/>
+      <c r="E11" s="101" t="s">
         <v>461</v>
       </c>
-      <c r="F11" s="103" t="s">
+      <c r="F11" s="112" t="s">
         <v>517</v>
       </c>
       <c r="G11" s="78"/>
-      <c r="H11" s="99"/>
+      <c r="H11" s="119"/>
       <c r="I11" s="53" t="s">
         <v>518</v>
       </c>
@@ -15232,20 +15703,20 @@
       <c r="K11" s="43" t="s">
         <v>519</v>
       </c>
-      <c r="L11" s="113"/>
-      <c r="M11" s="113"/>
+      <c r="L11" s="110"/>
+      <c r="M11" s="110"/>
     </row>
     <row r="12" spans="1:13" s="18" customFormat="1" ht="18" customHeight="1" thickBot="1">
-      <c r="A12" s="101"/>
-      <c r="B12" s="101"/>
-      <c r="C12" s="121"/>
-      <c r="D12" s="128"/>
-      <c r="E12" s="121"/>
-      <c r="F12" s="122"/>
+      <c r="A12" s="102"/>
+      <c r="B12" s="102"/>
+      <c r="C12" s="104"/>
+      <c r="D12" s="107"/>
+      <c r="E12" s="104"/>
+      <c r="F12" s="118"/>
       <c r="G12" s="80" t="s">
         <v>582</v>
       </c>
-      <c r="H12" s="123"/>
+      <c r="H12" s="120"/>
       <c r="I12" s="54" t="s">
         <v>520</v>
       </c>
@@ -15253,16 +15724,16 @@
       <c r="K12" s="56" t="s">
         <v>521</v>
       </c>
-      <c r="L12" s="113"/>
-      <c r="M12" s="113"/>
+      <c r="L12" s="110"/>
+      <c r="M12" s="110"/>
     </row>
     <row r="13" spans="1:13" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A13" s="101"/>
-      <c r="B13" s="101"/>
-      <c r="C13" s="101" t="s">
+      <c r="A13" s="102"/>
+      <c r="B13" s="102"/>
+      <c r="C13" s="102" t="s">
         <v>462</v>
       </c>
-      <c r="D13" s="116" t="s">
+      <c r="D13" s="106" t="s">
         <v>522</v>
       </c>
       <c r="E13" s="57" t="s">
@@ -15284,14 +15755,14 @@
       <c r="K13" s="51" t="s">
         <v>526</v>
       </c>
-      <c r="L13" s="113"/>
-      <c r="M13" s="113"/>
+      <c r="L13" s="110"/>
+      <c r="M13" s="110"/>
     </row>
     <row r="14" spans="1:13" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A14" s="101"/>
-      <c r="B14" s="101"/>
-      <c r="C14" s="101"/>
-      <c r="D14" s="116"/>
+      <c r="A14" s="102"/>
+      <c r="B14" s="102"/>
+      <c r="C14" s="102"/>
+      <c r="D14" s="106"/>
       <c r="E14" s="41" t="s">
         <v>464</v>
       </c>
@@ -15311,14 +15782,14 @@
       <c r="K14" s="43" t="s">
         <v>530</v>
       </c>
-      <c r="L14" s="113"/>
-      <c r="M14" s="113"/>
+      <c r="L14" s="110"/>
+      <c r="M14" s="110"/>
     </row>
     <row r="15" spans="1:13" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A15" s="101"/>
-      <c r="B15" s="101"/>
-      <c r="C15" s="101"/>
-      <c r="D15" s="116"/>
+      <c r="A15" s="102"/>
+      <c r="B15" s="102"/>
+      <c r="C15" s="102"/>
+      <c r="D15" s="106"/>
       <c r="E15" s="41" t="s">
         <v>465</v>
       </c>
@@ -15338,56 +15809,56 @@
       <c r="K15" s="43" t="s">
         <v>534</v>
       </c>
-      <c r="L15" s="113"/>
-      <c r="M15" s="113"/>
+      <c r="L15" s="110"/>
+      <c r="M15" s="110"/>
     </row>
     <row r="16" spans="1:13" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A16" s="101"/>
-      <c r="B16" s="101"/>
-      <c r="C16" s="101"/>
-      <c r="D16" s="116"/>
-      <c r="E16" s="100" t="s">
+      <c r="A16" s="102"/>
+      <c r="B16" s="102"/>
+      <c r="C16" s="102"/>
+      <c r="D16" s="106"/>
+      <c r="E16" s="101" t="s">
         <v>467</v>
       </c>
-      <c r="F16" s="103" t="s">
+      <c r="F16" s="112" t="s">
         <v>535</v>
       </c>
       <c r="G16" s="78"/>
-      <c r="H16" s="124"/>
+      <c r="H16" s="121"/>
       <c r="I16" s="63" t="s">
         <v>536</v>
       </c>
       <c r="J16" s="46"/>
       <c r="K16" s="43"/>
-      <c r="L16" s="113"/>
-      <c r="M16" s="113"/>
+      <c r="L16" s="110"/>
+      <c r="M16" s="110"/>
     </row>
     <row r="17" spans="1:14" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A17" s="101"/>
-      <c r="B17" s="101"/>
-      <c r="C17" s="101"/>
-      <c r="D17" s="116"/>
-      <c r="E17" s="101"/>
-      <c r="F17" s="104"/>
+      <c r="A17" s="102"/>
+      <c r="B17" s="102"/>
+      <c r="C17" s="102"/>
+      <c r="D17" s="106"/>
+      <c r="E17" s="102"/>
+      <c r="F17" s="113"/>
       <c r="G17" s="79"/>
-      <c r="H17" s="124"/>
+      <c r="H17" s="121"/>
       <c r="I17" s="63" t="s">
         <v>537</v>
       </c>
       <c r="J17" s="46"/>
       <c r="K17" s="43"/>
-      <c r="L17" s="113"/>
-      <c r="M17" s="113"/>
+      <c r="L17" s="110"/>
+      <c r="M17" s="110"/>
     </row>
     <row r="18" spans="1:14" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A18" s="101"/>
-      <c r="B18" s="101"/>
-      <c r="C18" s="101"/>
-      <c r="D18" s="116"/>
-      <c r="E18" s="101"/>
-      <c r="F18" s="104"/>
+      <c r="A18" s="102"/>
+      <c r="B18" s="102"/>
+      <c r="C18" s="102"/>
+      <c r="D18" s="106"/>
+      <c r="E18" s="102"/>
+      <c r="F18" s="113"/>
       <c r="G18" s="79"/>
-      <c r="H18" s="124"/>
+      <c r="H18" s="121"/>
       <c r="I18" s="43" t="s">
         <v>538</v>
       </c>
@@ -15395,18 +15866,18 @@
       <c r="K18" s="63" t="s">
         <v>539</v>
       </c>
-      <c r="L18" s="113"/>
-      <c r="M18" s="113"/>
+      <c r="L18" s="110"/>
+      <c r="M18" s="110"/>
     </row>
     <row r="19" spans="1:14" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A19" s="101"/>
-      <c r="B19" s="101"/>
-      <c r="C19" s="101"/>
-      <c r="D19" s="116"/>
-      <c r="E19" s="101"/>
-      <c r="F19" s="104"/>
+      <c r="A19" s="102"/>
+      <c r="B19" s="102"/>
+      <c r="C19" s="102"/>
+      <c r="D19" s="106"/>
+      <c r="E19" s="102"/>
+      <c r="F19" s="113"/>
       <c r="G19" s="79"/>
-      <c r="H19" s="124"/>
+      <c r="H19" s="121"/>
       <c r="I19" s="43" t="s">
         <v>540</v>
       </c>
@@ -15414,18 +15885,18 @@
       <c r="K19" s="63" t="s">
         <v>541</v>
       </c>
-      <c r="L19" s="113"/>
-      <c r="M19" s="113"/>
+      <c r="L19" s="110"/>
+      <c r="M19" s="110"/>
     </row>
     <row r="20" spans="1:14" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
-      <c r="C20" s="101"/>
-      <c r="D20" s="116"/>
-      <c r="E20" s="101"/>
-      <c r="F20" s="104"/>
+      <c r="A20" s="102"/>
+      <c r="B20" s="102"/>
+      <c r="C20" s="102"/>
+      <c r="D20" s="106"/>
+      <c r="E20" s="102"/>
+      <c r="F20" s="113"/>
       <c r="G20" s="79"/>
-      <c r="H20" s="124"/>
+      <c r="H20" s="121"/>
       <c r="I20" s="43" t="s">
         <v>542</v>
       </c>
@@ -15433,44 +15904,44 @@
       <c r="K20" s="63" t="s">
         <v>543</v>
       </c>
-      <c r="L20" s="113"/>
-      <c r="M20" s="113"/>
+      <c r="L20" s="110"/>
+      <c r="M20" s="110"/>
     </row>
     <row r="21" spans="1:14" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
-      <c r="C21" s="101"/>
-      <c r="D21" s="116"/>
-      <c r="E21" s="101"/>
-      <c r="F21" s="104"/>
+      <c r="A21" s="102"/>
+      <c r="B21" s="102"/>
+      <c r="C21" s="102"/>
+      <c r="D21" s="106"/>
+      <c r="E21" s="102"/>
+      <c r="F21" s="113"/>
       <c r="G21" s="79"/>
-      <c r="H21" s="124"/>
+      <c r="H21" s="121"/>
       <c r="I21" s="45" t="s">
         <v>484</v>
       </c>
       <c r="J21" s="46"/>
       <c r="K21" s="63"/>
-      <c r="L21" s="113"/>
-      <c r="M21" s="113"/>
+      <c r="L21" s="110"/>
+      <c r="M21" s="110"/>
     </row>
     <row r="22" spans="1:14" s="18" customFormat="1" ht="23" customHeight="1">
-      <c r="A22" s="102"/>
-      <c r="B22" s="102"/>
-      <c r="C22" s="102"/>
-      <c r="D22" s="117"/>
-      <c r="E22" s="102"/>
-      <c r="F22" s="105"/>
+      <c r="A22" s="103"/>
+      <c r="B22" s="103"/>
+      <c r="C22" s="103"/>
+      <c r="D22" s="108"/>
+      <c r="E22" s="103"/>
+      <c r="F22" s="114"/>
       <c r="G22" s="58" t="s">
         <v>582</v>
       </c>
-      <c r="H22" s="124"/>
+      <c r="H22" s="121"/>
       <c r="I22" s="43" t="s">
         <v>544</v>
       </c>
       <c r="J22" s="46"/>
       <c r="K22" s="44"/>
-      <c r="L22" s="114"/>
-      <c r="M22" s="114"/>
+      <c r="L22" s="111"/>
+      <c r="M22" s="111"/>
     </row>
     <row r="23" spans="1:14" s="18" customFormat="1" ht="8" customHeight="1">
       <c r="A23" s="64"/>
@@ -15488,26 +15959,26 @@
       <c r="M23" s="69"/>
     </row>
     <row r="24" spans="1:14" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A24" s="100" t="s">
+      <c r="A24" s="101" t="s">
         <v>468</v>
       </c>
-      <c r="B24" s="118" t="s">
+      <c r="B24" s="122" t="s">
         <v>469</v>
       </c>
-      <c r="C24" s="100" t="s">
+      <c r="C24" s="101" t="s">
         <v>470</v>
       </c>
-      <c r="D24" s="115" t="s">
+      <c r="D24" s="105" t="s">
         <v>545</v>
       </c>
-      <c r="E24" s="100" t="s">
+      <c r="E24" s="101" t="s">
         <v>471</v>
       </c>
-      <c r="F24" s="103" t="s">
+      <c r="F24" s="112" t="s">
         <v>546</v>
       </c>
       <c r="G24" s="78"/>
-      <c r="H24" s="106" t="s">
+      <c r="H24" s="115" t="s">
         <v>547</v>
       </c>
       <c r="I24" s="44" t="s">
@@ -15519,47 +15990,47 @@
       <c r="K24" s="43" t="s">
         <v>548</v>
       </c>
-      <c r="L24" s="112" t="s">
+      <c r="L24" s="109" t="s">
         <v>507</v>
       </c>
-      <c r="M24" s="99" t="s">
+      <c r="M24" s="119" t="s">
         <v>474</v>
       </c>
       <c r="N24" s="47"/>
     </row>
     <row r="25" spans="1:14" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A25" s="101"/>
-      <c r="B25" s="119"/>
-      <c r="C25" s="101"/>
-      <c r="D25" s="116"/>
-      <c r="E25" s="102"/>
-      <c r="F25" s="105"/>
+      <c r="A25" s="102"/>
+      <c r="B25" s="123"/>
+      <c r="C25" s="102"/>
+      <c r="D25" s="106"/>
+      <c r="E25" s="103"/>
+      <c r="F25" s="114"/>
       <c r="G25" s="58" t="s">
         <v>582</v>
       </c>
-      <c r="H25" s="108"/>
+      <c r="H25" s="117"/>
       <c r="I25" s="44" t="s">
         <v>549</v>
       </c>
       <c r="J25" s="45"/>
       <c r="K25" s="43"/>
-      <c r="L25" s="113"/>
-      <c r="M25" s="99"/>
+      <c r="L25" s="110"/>
+      <c r="M25" s="119"/>
       <c r="N25" s="47"/>
     </row>
     <row r="26" spans="1:14" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A26" s="101"/>
-      <c r="B26" s="119"/>
-      <c r="C26" s="101"/>
-      <c r="D26" s="116"/>
-      <c r="E26" s="100" t="s">
+      <c r="A26" s="102"/>
+      <c r="B26" s="123"/>
+      <c r="C26" s="102"/>
+      <c r="D26" s="106"/>
+      <c r="E26" s="101" t="s">
         <v>475</v>
       </c>
-      <c r="F26" s="103" t="s">
+      <c r="F26" s="112" t="s">
         <v>550</v>
       </c>
       <c r="G26" s="78"/>
-      <c r="H26" s="106" t="s">
+      <c r="H26" s="115" t="s">
         <v>551</v>
       </c>
       <c r="I26" s="44" t="s">
@@ -15571,21 +16042,21 @@
       <c r="K26" s="43" t="s">
         <v>553</v>
       </c>
-      <c r="L26" s="113"/>
-      <c r="M26" s="99"/>
+      <c r="L26" s="110"/>
+      <c r="M26" s="119"/>
       <c r="N26" s="47"/>
     </row>
     <row r="27" spans="1:14" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A27" s="101"/>
-      <c r="B27" s="119"/>
-      <c r="C27" s="101"/>
-      <c r="D27" s="116"/>
-      <c r="E27" s="102"/>
-      <c r="F27" s="105"/>
+      <c r="A27" s="102"/>
+      <c r="B27" s="123"/>
+      <c r="C27" s="102"/>
+      <c r="D27" s="106"/>
+      <c r="E27" s="103"/>
+      <c r="F27" s="114"/>
       <c r="G27" s="58" t="s">
         <v>583</v>
       </c>
-      <c r="H27" s="108"/>
+      <c r="H27" s="117"/>
       <c r="I27" s="44" t="s">
         <v>483</v>
       </c>
@@ -15593,15 +16064,15 @@
         <v>479</v>
       </c>
       <c r="K27" s="43"/>
-      <c r="L27" s="113"/>
-      <c r="M27" s="99"/>
+      <c r="L27" s="110"/>
+      <c r="M27" s="119"/>
       <c r="N27" s="47"/>
     </row>
     <row r="28" spans="1:14" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A28" s="101"/>
-      <c r="B28" s="119"/>
-      <c r="C28" s="101"/>
-      <c r="D28" s="116"/>
+      <c r="A28" s="102"/>
+      <c r="B28" s="123"/>
+      <c r="C28" s="102"/>
+      <c r="D28" s="106"/>
       <c r="E28" s="41" t="s">
         <v>477</v>
       </c>
@@ -15620,15 +16091,15 @@
       <c r="K28" s="43" t="s">
         <v>556</v>
       </c>
-      <c r="L28" s="113"/>
-      <c r="M28" s="99"/>
+      <c r="L28" s="110"/>
+      <c r="M28" s="119"/>
       <c r="N28" s="47"/>
     </row>
     <row r="29" spans="1:14" s="18" customFormat="1" ht="19" customHeight="1">
-      <c r="A29" s="102"/>
-      <c r="B29" s="120"/>
-      <c r="C29" s="102"/>
-      <c r="D29" s="117"/>
+      <c r="A29" s="103"/>
+      <c r="B29" s="124"/>
+      <c r="C29" s="103"/>
+      <c r="D29" s="108"/>
       <c r="E29" s="41" t="s">
         <v>480</v>
       </c>
@@ -15650,8 +16121,8 @@
       <c r="K29" s="43" t="s">
         <v>559</v>
       </c>
-      <c r="L29" s="114"/>
-      <c r="M29" s="99"/>
+      <c r="L29" s="111"/>
+      <c r="M29" s="119"/>
       <c r="N29" s="47"/>
     </row>
     <row r="30" spans="1:14" s="18" customFormat="1" ht="8" customHeight="1">
@@ -15670,26 +16141,26 @@
       <c r="M30" s="69"/>
     </row>
     <row r="31" spans="1:14" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A31" s="100" t="s">
+      <c r="A31" s="101" t="s">
         <v>485</v>
       </c>
-      <c r="B31" s="100" t="s">
+      <c r="B31" s="101" t="s">
         <v>486</v>
       </c>
-      <c r="C31" s="100" t="s">
+      <c r="C31" s="101" t="s">
         <v>487</v>
       </c>
-      <c r="D31" s="115" t="s">
+      <c r="D31" s="105" t="s">
         <v>560</v>
       </c>
-      <c r="E31" s="100" t="s">
+      <c r="E31" s="101" t="s">
         <v>488</v>
       </c>
-      <c r="F31" s="103" t="s">
+      <c r="F31" s="112" t="s">
         <v>561</v>
       </c>
       <c r="G31" s="78"/>
-      <c r="H31" s="106" t="s">
+      <c r="H31" s="115" t="s">
         <v>562</v>
       </c>
       <c r="I31" s="76" t="s">
@@ -15701,22 +16172,22 @@
       <c r="K31" s="43" t="s">
         <v>564</v>
       </c>
-      <c r="L31" s="99" t="s">
+      <c r="L31" s="119" t="s">
         <v>490</v>
       </c>
-      <c r="M31" s="99" t="s">
+      <c r="M31" s="119" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="32" spans="1:14" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A32" s="101"/>
-      <c r="B32" s="101"/>
-      <c r="C32" s="101"/>
-      <c r="D32" s="116"/>
-      <c r="E32" s="101"/>
-      <c r="F32" s="104"/>
+      <c r="A32" s="102"/>
+      <c r="B32" s="102"/>
+      <c r="C32" s="102"/>
+      <c r="D32" s="106"/>
+      <c r="E32" s="102"/>
+      <c r="F32" s="113"/>
       <c r="G32" s="79"/>
-      <c r="H32" s="107"/>
+      <c r="H32" s="116"/>
       <c r="I32" s="51" t="s">
         <v>565</v>
       </c>
@@ -15724,79 +16195,79 @@
       <c r="K32" s="43" t="s">
         <v>566</v>
       </c>
-      <c r="L32" s="99"/>
-      <c r="M32" s="99"/>
+      <c r="L32" s="119"/>
+      <c r="M32" s="119"/>
     </row>
     <row r="33" spans="1:13" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A33" s="101"/>
-      <c r="B33" s="101"/>
-      <c r="C33" s="101"/>
-      <c r="D33" s="116"/>
-      <c r="E33" s="102"/>
-      <c r="F33" s="105"/>
+      <c r="A33" s="102"/>
+      <c r="B33" s="102"/>
+      <c r="C33" s="102"/>
+      <c r="D33" s="106"/>
+      <c r="E33" s="103"/>
+      <c r="F33" s="114"/>
       <c r="G33" s="58" t="s">
         <v>582</v>
       </c>
-      <c r="H33" s="108"/>
+      <c r="H33" s="117"/>
       <c r="I33" s="51" t="s">
         <v>500</v>
       </c>
       <c r="J33" s="44"/>
       <c r="K33" s="43"/>
-      <c r="L33" s="99"/>
-      <c r="M33" s="99"/>
+      <c r="L33" s="119"/>
+      <c r="M33" s="119"/>
     </row>
     <row r="34" spans="1:13" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A34" s="101"/>
-      <c r="B34" s="101"/>
-      <c r="C34" s="101"/>
-      <c r="D34" s="116"/>
-      <c r="E34" s="100" t="s">
+      <c r="A34" s="102"/>
+      <c r="B34" s="102"/>
+      <c r="C34" s="102"/>
+      <c r="D34" s="106"/>
+      <c r="E34" s="101" t="s">
         <v>492</v>
       </c>
-      <c r="F34" s="103" t="s">
+      <c r="F34" s="112" t="s">
         <v>567</v>
       </c>
       <c r="G34" s="78"/>
-      <c r="H34" s="106" t="s">
+      <c r="H34" s="115" t="s">
         <v>568</v>
       </c>
       <c r="I34" s="44" t="s">
         <v>569</v>
       </c>
       <c r="J34" s="44"/>
-      <c r="K34" s="109"/>
-      <c r="L34" s="99"/>
-      <c r="M34" s="99"/>
+      <c r="K34" s="125"/>
+      <c r="L34" s="119"/>
+      <c r="M34" s="119"/>
     </row>
     <row r="35" spans="1:13" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A35" s="101"/>
-      <c r="B35" s="101"/>
-      <c r="C35" s="101"/>
-      <c r="D35" s="116"/>
-      <c r="E35" s="101"/>
-      <c r="F35" s="104"/>
+      <c r="A35" s="102"/>
+      <c r="B35" s="102"/>
+      <c r="C35" s="102"/>
+      <c r="D35" s="106"/>
+      <c r="E35" s="102"/>
+      <c r="F35" s="113"/>
       <c r="G35" s="79"/>
-      <c r="H35" s="107"/>
+      <c r="H35" s="116"/>
       <c r="I35" s="44" t="s">
         <v>496</v>
       </c>
       <c r="J35" s="44"/>
-      <c r="K35" s="109"/>
-      <c r="L35" s="99"/>
-      <c r="M35" s="99"/>
+      <c r="K35" s="125"/>
+      <c r="L35" s="119"/>
+      <c r="M35" s="119"/>
     </row>
     <row r="36" spans="1:13" s="18" customFormat="1" ht="14" customHeight="1">
-      <c r="A36" s="101"/>
-      <c r="B36" s="101"/>
-      <c r="C36" s="101"/>
-      <c r="D36" s="116"/>
-      <c r="E36" s="102"/>
-      <c r="F36" s="105"/>
+      <c r="A36" s="102"/>
+      <c r="B36" s="102"/>
+      <c r="C36" s="102"/>
+      <c r="D36" s="106"/>
+      <c r="E36" s="103"/>
+      <c r="F36" s="114"/>
       <c r="G36" s="58" t="s">
         <v>582</v>
       </c>
-      <c r="H36" s="108"/>
+      <c r="H36" s="117"/>
       <c r="I36" s="44" t="s">
         <v>570</v>
       </c>
@@ -15806,68 +16277,68 @@
       <c r="K36" s="43" t="s">
         <v>494</v>
       </c>
-      <c r="L36" s="99"/>
-      <c r="M36" s="99"/>
+      <c r="L36" s="119"/>
+      <c r="M36" s="119"/>
     </row>
     <row r="37" spans="1:13" s="18" customFormat="1" ht="18" customHeight="1">
-      <c r="A37" s="101"/>
-      <c r="B37" s="101"/>
-      <c r="C37" s="101"/>
-      <c r="D37" s="116"/>
-      <c r="E37" s="100" t="s">
+      <c r="A37" s="102"/>
+      <c r="B37" s="102"/>
+      <c r="C37" s="102"/>
+      <c r="D37" s="106"/>
+      <c r="E37" s="101" t="s">
         <v>495</v>
       </c>
-      <c r="F37" s="103" t="s">
+      <c r="F37" s="112" t="s">
         <v>571</v>
       </c>
       <c r="G37" s="78"/>
-      <c r="H37" s="110" t="s">
+      <c r="H37" s="126" t="s">
         <v>572</v>
       </c>
       <c r="I37" s="44" t="s">
         <v>573</v>
       </c>
-      <c r="J37" s="111" t="s">
+      <c r="J37" s="127" t="s">
         <v>497</v>
       </c>
-      <c r="K37" s="110" t="s">
+      <c r="K37" s="126" t="s">
         <v>499</v>
       </c>
-      <c r="L37" s="99"/>
-      <c r="M37" s="99"/>
+      <c r="L37" s="119"/>
+      <c r="M37" s="119"/>
     </row>
     <row r="38" spans="1:13" s="18" customFormat="1" ht="18" customHeight="1">
-      <c r="A38" s="101"/>
-      <c r="B38" s="101"/>
-      <c r="C38" s="101"/>
-      <c r="D38" s="116"/>
-      <c r="E38" s="101"/>
-      <c r="F38" s="104"/>
+      <c r="A38" s="102"/>
+      <c r="B38" s="102"/>
+      <c r="C38" s="102"/>
+      <c r="D38" s="106"/>
+      <c r="E38" s="102"/>
+      <c r="F38" s="113"/>
       <c r="G38" s="79" t="s">
         <v>582</v>
       </c>
-      <c r="H38" s="110"/>
+      <c r="H38" s="126"/>
       <c r="I38" s="63" t="s">
         <v>574</v>
       </c>
-      <c r="J38" s="111"/>
-      <c r="K38" s="110"/>
-      <c r="L38" s="99"/>
-      <c r="M38" s="99"/>
+      <c r="J38" s="127"/>
+      <c r="K38" s="126"/>
+      <c r="L38" s="119"/>
+      <c r="M38" s="119"/>
     </row>
     <row r="39" spans="1:13" s="18" customFormat="1" ht="18" customHeight="1">
-      <c r="A39" s="101"/>
-      <c r="B39" s="101"/>
-      <c r="C39" s="101"/>
-      <c r="D39" s="116"/>
-      <c r="E39" s="101" t="s">
+      <c r="A39" s="102"/>
+      <c r="B39" s="102"/>
+      <c r="C39" s="102"/>
+      <c r="D39" s="106"/>
+      <c r="E39" s="102" t="s">
         <v>498</v>
       </c>
-      <c r="F39" s="104" t="s">
+      <c r="F39" s="113" t="s">
         <v>575</v>
       </c>
       <c r="G39" s="79"/>
-      <c r="H39" s="110" t="s">
+      <c r="H39" s="126" t="s">
         <v>576</v>
       </c>
       <c r="I39" s="63" t="s">
@@ -15877,18 +16348,18 @@
       <c r="K39" s="51" t="s">
         <v>578</v>
       </c>
-      <c r="L39" s="99"/>
-      <c r="M39" s="99"/>
+      <c r="L39" s="119"/>
+      <c r="M39" s="119"/>
     </row>
     <row r="40" spans="1:13" s="18" customFormat="1" ht="18" customHeight="1">
-      <c r="A40" s="101"/>
-      <c r="B40" s="101"/>
-      <c r="C40" s="101"/>
-      <c r="D40" s="116"/>
-      <c r="E40" s="101"/>
-      <c r="F40" s="104"/>
+      <c r="A40" s="102"/>
+      <c r="B40" s="102"/>
+      <c r="C40" s="102"/>
+      <c r="D40" s="106"/>
+      <c r="E40" s="102"/>
+      <c r="F40" s="113"/>
       <c r="G40" s="79"/>
-      <c r="H40" s="110"/>
+      <c r="H40" s="126"/>
       <c r="I40" s="63" t="s">
         <v>579</v>
       </c>
@@ -15896,27 +16367,27 @@
       <c r="K40" s="51" t="s">
         <v>580</v>
       </c>
-      <c r="L40" s="99"/>
-      <c r="M40" s="99"/>
+      <c r="L40" s="119"/>
+      <c r="M40" s="119"/>
     </row>
     <row r="41" spans="1:13" s="18" customFormat="1" ht="17" customHeight="1">
-      <c r="A41" s="102"/>
-      <c r="B41" s="102"/>
-      <c r="C41" s="102"/>
-      <c r="D41" s="117"/>
-      <c r="E41" s="102"/>
-      <c r="F41" s="105"/>
+      <c r="A41" s="103"/>
+      <c r="B41" s="103"/>
+      <c r="C41" s="103"/>
+      <c r="D41" s="108"/>
+      <c r="E41" s="103"/>
+      <c r="F41" s="114"/>
       <c r="G41" s="58" t="s">
         <v>582</v>
       </c>
-      <c r="H41" s="110"/>
+      <c r="H41" s="126"/>
       <c r="I41" s="63" t="s">
         <v>581</v>
       </c>
       <c r="J41" s="46"/>
       <c r="K41" s="43"/>
-      <c r="L41" s="99"/>
-      <c r="M41" s="99"/>
+      <c r="L41" s="119"/>
+      <c r="M41" s="119"/>
     </row>
     <row r="42" spans="1:13">
       <c r="K42" s="77"/>
@@ -15924,42 +16395,6 @@
     <row r="43" spans="1:13" ht="23" customHeight="1"/>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F4"/>
-    <mergeCell ref="A6:A22"/>
-    <mergeCell ref="B6:B22"/>
-    <mergeCell ref="C6:C12"/>
-    <mergeCell ref="D6:D12"/>
-    <mergeCell ref="C13:C22"/>
-    <mergeCell ref="D13:D22"/>
-    <mergeCell ref="L6:L22"/>
-    <mergeCell ref="M6:M22"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="E16:E22"/>
-    <mergeCell ref="F16:F22"/>
-    <mergeCell ref="H16:H22"/>
-    <mergeCell ref="A24:A29"/>
-    <mergeCell ref="B24:B29"/>
-    <mergeCell ref="C24:C29"/>
-    <mergeCell ref="D24:D29"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="A31:A41"/>
-    <mergeCell ref="B31:B41"/>
-    <mergeCell ref="C31:C41"/>
-    <mergeCell ref="D31:D41"/>
-    <mergeCell ref="E31:E33"/>
-    <mergeCell ref="L24:L29"/>
-    <mergeCell ref="M24:M29"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="H24:H25"/>
     <mergeCell ref="L31:L41"/>
     <mergeCell ref="M31:M41"/>
     <mergeCell ref="E34:E36"/>
@@ -15976,6 +16411,42 @@
     <mergeCell ref="H39:H41"/>
     <mergeCell ref="F31:F33"/>
     <mergeCell ref="H31:H33"/>
+    <mergeCell ref="L24:L29"/>
+    <mergeCell ref="M24:M29"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="A31:A41"/>
+    <mergeCell ref="B31:B41"/>
+    <mergeCell ref="C31:C41"/>
+    <mergeCell ref="D31:D41"/>
+    <mergeCell ref="E31:E33"/>
+    <mergeCell ref="A24:A29"/>
+    <mergeCell ref="B24:B29"/>
+    <mergeCell ref="C24:C29"/>
+    <mergeCell ref="D24:D29"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="L6:L22"/>
+    <mergeCell ref="M6:M22"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="E16:E22"/>
+    <mergeCell ref="F16:F22"/>
+    <mergeCell ref="H16:H22"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F4"/>
+    <mergeCell ref="A6:A22"/>
+    <mergeCell ref="B6:B22"/>
+    <mergeCell ref="C6:C12"/>
+    <mergeCell ref="D6:D12"/>
+    <mergeCell ref="C13:C22"/>
+    <mergeCell ref="D13:D22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H6" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>

</xml_diff>